<commit_message>
[ADD] face Counter & only one face
</commit_message>
<xml_diff>
--- a/main/parkslockup/parkslockup/user.xlsx
+++ b/main/parkslockup/parkslockup/user.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DX2"/>
+  <dimension ref="A1:DX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,392 +807,6 @@
         <v>0.01923026889562607</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>-0.06585553288459778</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.03074822574853897</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0508991926908493</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.09837181866168976</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-0.1256058812141418</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.050654336810112</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-0.07512503117322922</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-0.07811924815177917</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.03589428961277008</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.1257051229476929</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.1550488471984863</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-0.09024935960769653</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-0.1628322601318359</v>
-      </c>
-      <c r="N2" t="n">
-        <v>-0.0599595233798027</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-0.07140208780765533</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.1569103300571442</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>-0.07934436202049255</v>
-      </c>
-      <c r="R2" t="n">
-        <v>-0.07767032086849213</v>
-      </c>
-      <c r="S2" t="n">
-        <v>-0.04432963207364082</v>
-      </c>
-      <c r="T2" t="n">
-        <v>-0.02578068524599075</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.1065509766340256</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.05830461904406548</v>
-      </c>
-      <c r="W2" t="n">
-        <v>-0.04470650106668472</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.02722255140542984</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>-0.06110879778862</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>-0.2336134165525436</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>-0.08894574642181396</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>-0.01149528473615646</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.03656462207436562</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>-0.04717196524143219</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>-0.06297218799591064</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.09532672911882401</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>-0.166898638010025</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>-0.03715885430574417</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.03658526390790939</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.1295772790908813</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>-0.03265073150396347</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>-0.04881024360656738</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.1113771349191666</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>-0.005085961893200874</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>-0.2271403074264526</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.07518266141414642</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.05796873569488525</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.2310905158519745</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.1676008701324463</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0.03717324882745743</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0.02361865900456905</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>-0.1147288382053375</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0.1086830198764801</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>-0.1720506101846695</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>0.04533839598298073</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>0.1359201371669769</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0.1192809790372849</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.07950903475284576</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>0.01048281043767929</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>-0.1206666827201843</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0.06973680853843689</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0.1113423407077789</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>-0.07813864201307297</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>0.0509672723710537</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>0.1117683500051498</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>-0.05528856441378593</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0.004256298765540123</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>-0.09570624679327011</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0.1972243785858154</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>0.03965331614017487</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>-0.1237938106060028</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>-0.1699121445417404</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>0.1101763546466827</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>-0.1473391354084015</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>-0.1263187527656555</v>
-      </c>
-      <c r="BT2" t="n">
-        <v>0.05209267884492874</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>-0.1422167718410492</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>-0.1279003620147705</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>-0.2776837646961212</v>
-      </c>
-      <c r="BX2" t="n">
-        <v>0.04449312388896942</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>0.2996753752231598</v>
-      </c>
-      <c r="BZ2" t="n">
-        <v>0.1534487903118134</v>
-      </c>
-      <c r="CA2" t="n">
-        <v>-0.2066330462694168</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>0.07631427049636841</v>
-      </c>
-      <c r="CC2" t="n">
-        <v>-0.03490406274795532</v>
-      </c>
-      <c r="CD2" t="n">
-        <v>0.07661205530166626</v>
-      </c>
-      <c r="CE2" t="n">
-        <v>0.1757135689258575</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>0.1088935136795044</v>
-      </c>
-      <c r="CG2" t="n">
-        <v>-0.02960297465324402</v>
-      </c>
-      <c r="CH2" t="n">
-        <v>0.02726239711046219</v>
-      </c>
-      <c r="CI2" t="n">
-        <v>-0.04233066737651825</v>
-      </c>
-      <c r="CJ2" t="n">
-        <v>-0.0231374055147171</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>0.2449500560760498</v>
-      </c>
-      <c r="CL2" t="n">
-        <v>-0.09091836214065552</v>
-      </c>
-      <c r="CM2" t="n">
-        <v>-0.04551728069782257</v>
-      </c>
-      <c r="CN2" t="n">
-        <v>0.201474204659462</v>
-      </c>
-      <c r="CO2" t="n">
-        <v>0.03396333381533623</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>0.0775834321975708</v>
-      </c>
-      <c r="CQ2" t="n">
-        <v>0.01252308860421181</v>
-      </c>
-      <c r="CR2" t="n">
-        <v>-0.005289569497108459</v>
-      </c>
-      <c r="CS2" t="n">
-        <v>-0.003711163997650146</v>
-      </c>
-      <c r="CT2" t="n">
-        <v>0.02477498725056648</v>
-      </c>
-      <c r="CU2" t="n">
-        <v>-0.09873155504465103</v>
-      </c>
-      <c r="CV2" t="n">
-        <v>0.03414099663496017</v>
-      </c>
-      <c r="CW2" t="n">
-        <v>0.08426769077777863</v>
-      </c>
-      <c r="CX2" t="n">
-        <v>-0.1292830109596252</v>
-      </c>
-      <c r="CY2" t="n">
-        <v>-0.004707157611846924</v>
-      </c>
-      <c r="CZ2" t="n">
-        <v>0.1415034532546997</v>
-      </c>
-      <c r="DA2" t="n">
-        <v>-0.1736684441566467</v>
-      </c>
-      <c r="DB2" t="n">
-        <v>0.1658155918121338</v>
-      </c>
-      <c r="DC2" t="n">
-        <v>-0.02425876259803772</v>
-      </c>
-      <c r="DD2" t="n">
-        <v>0.0887603834271431</v>
-      </c>
-      <c r="DE2" t="n">
-        <v>0.04371903836727142</v>
-      </c>
-      <c r="DF2" t="n">
-        <v>0.04471378028392792</v>
-      </c>
-      <c r="DG2" t="n">
-        <v>-0.1425651758909225</v>
-      </c>
-      <c r="DH2" t="n">
-        <v>-0.01781892776489258</v>
-      </c>
-      <c r="DI2" t="n">
-        <v>0.1286093443632126</v>
-      </c>
-      <c r="DJ2" t="n">
-        <v>-0.1987634599208832</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>0.2446770370006561</v>
-      </c>
-      <c r="DL2" t="n">
-        <v>0.1955911070108414</v>
-      </c>
-      <c r="DM2" t="n">
-        <v>0.06502199172973633</v>
-      </c>
-      <c r="DN2" t="n">
-        <v>0.06458475440740585</v>
-      </c>
-      <c r="DO2" t="n">
-        <v>0.2150526344776154</v>
-      </c>
-      <c r="DP2" t="n">
-        <v>0.1104782968759537</v>
-      </c>
-      <c r="DQ2" t="n">
-        <v>0.03593744337558746</v>
-      </c>
-      <c r="DR2" t="n">
-        <v>-0.03070724755525589</v>
-      </c>
-      <c r="DS2" t="n">
-        <v>-0.1536105871200562</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>-0.07392101734876633</v>
-      </c>
-      <c r="DU2" t="n">
-        <v>0.1414052993059158</v>
-      </c>
-      <c r="DV2" t="n">
-        <v>-0.02991615235805511</v>
-      </c>
-      <c r="DW2" t="n">
-        <v>0.05995562672615051</v>
-      </c>
-      <c r="DX2" t="n">
-        <v>0.03869921714067459</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] regist imgs by imgs dir path
</commit_message>
<xml_diff>
--- a/main/parkslockup/parkslockup/user.xlsx
+++ b/main/parkslockup/parkslockup/user.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DX1"/>
+  <dimension ref="A1:DX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +807,392 @@
         <v>0.01923026889562607</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-0.1730910390615463</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0468733087182045</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.02230261638760567</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.1236186027526855</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.1355118155479431</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.004758149385452271</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-0.04674947634339333</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.08549851924180984</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.06096422672271729</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.1456707864999771</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.1873953938484192</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.05990472063422203</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.2161078751087189</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.07083684206008911</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.05230434238910675</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.1688528507947922</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.10996925085783</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-0.1554861068725586</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-0.06284290552139282</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.01328445971012115</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.09919625520706177</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.06926415860652924</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-0.07293561846017838</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.03993618488311768</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-0.1648965626955032</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-0.2873676419258118</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>-0.09258896857500076</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.007343828678131104</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-0.08637028932571411</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-0.08937422931194305</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>-0.0372329093515873</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.05746649950742722</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>-0.1870715022087097</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.0144367516040802</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.04682070761919022</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.1388134360313416</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.01048935949802399</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>-0.01035474985837936</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.09950096905231476</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.04611104354262352</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>-0.2723390758037567</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.06730875372886658</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.1117917224764824</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.2708423733711243</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.2074048519134521</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>-0.002255335450172424</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>-0.01857819408178329</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>-0.1428809612989426</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.1252310872077942</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>-0.2293906360864639</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>-0.04201679304242134</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.1312595307826996</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.03448783606290817</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.03538764268159866</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>-0.004816927015781403</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>-0.09243146330118179</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.02554529905319214</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.1159960031509399</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>-0.1160740330815315</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.03537945449352264</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.06928659975528717</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>-0.1114377677440643</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>-0.08367887139320374</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>-0.1209922209382057</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.1632474362850189</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.03589450195431709</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>-0.1758359968662262</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>-0.2392930239439011</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0.08649689704179764</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>-0.1891351044178009</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>-0.1356927454471588</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0.1131480112671852</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>-0.1520384252071381</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>-0.2002529799938202</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>-0.3503864407539368</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0.03609529137611389</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>0.3386359214782715</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0.1422533094882965</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>-0.1987703293561935</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.08287635445594788</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>0.008811849169433117</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>0.04027725756168365</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>0.1274399161338806</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0.1737797409296036</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>0.007274281233549118</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0.06602674722671509</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>-0.08098559081554413</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0.06098867952823639</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.2891929149627686</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>-0.04164474457502365</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>-0.008886042982339859</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0.2377078533172607</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>0.02674798667430878</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>0.1161438524723053</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0.01022475212812424</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0.06723983585834503</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>-0.04888508468866348</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>-0.02901731431484222</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>-0.1517019271850586</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>0.003211945295333862</v>
+      </c>
+      <c r="CW2" t="n">
+        <v>0.04904887825250626</v>
+      </c>
+      <c r="CX2" t="n">
+        <v>-0.03636002540588379</v>
+      </c>
+      <c r="CY2" t="n">
+        <v>0.001870393753051758</v>
+      </c>
+      <c r="CZ2" t="n">
+        <v>0.1718954145908356</v>
+      </c>
+      <c r="DA2" t="n">
+        <v>-0.1269590258598328</v>
+      </c>
+      <c r="DB2" t="n">
+        <v>0.1904156804084778</v>
+      </c>
+      <c r="DC2" t="n">
+        <v>-0.0403340682387352</v>
+      </c>
+      <c r="DD2" t="n">
+        <v>0.03302508220076561</v>
+      </c>
+      <c r="DE2" t="n">
+        <v>-0.03621438145637512</v>
+      </c>
+      <c r="DF2" t="n">
+        <v>-0.03502778708934784</v>
+      </c>
+      <c r="DG2" t="n">
+        <v>-0.07337862998247147</v>
+      </c>
+      <c r="DH2" t="n">
+        <v>0.005858689546585083</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>0.08885832130908966</v>
+      </c>
+      <c r="DJ2" t="n">
+        <v>-0.2003527730703354</v>
+      </c>
+      <c r="DK2" t="n">
+        <v>0.1659952402114868</v>
+      </c>
+      <c r="DL2" t="n">
+        <v>0.2087558507919312</v>
+      </c>
+      <c r="DM2" t="n">
+        <v>0.08905559778213501</v>
+      </c>
+      <c r="DN2" t="n">
+        <v>0.03161385282874107</v>
+      </c>
+      <c r="DO2" t="n">
+        <v>0.1914173662662506</v>
+      </c>
+      <c r="DP2" t="n">
+        <v>-0.002605810761451721</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>-0.005448907613754272</v>
+      </c>
+      <c r="DR2" t="n">
+        <v>0.03450989723205566</v>
+      </c>
+      <c r="DS2" t="n">
+        <v>-0.2104713171720505</v>
+      </c>
+      <c r="DT2" t="n">
+        <v>-0.03083633072674274</v>
+      </c>
+      <c r="DU2" t="n">
+        <v>0.09877301007509232</v>
+      </c>
+      <c r="DV2" t="n">
+        <v>-0.1010307371616364</v>
+      </c>
+      <c r="DW2" t="n">
+        <v>0.09877075254917145</v>
+      </c>
+      <c r="DX2" t="n">
+        <v>-0.04287730902433395</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] clear duty in encoding
</commit_message>
<xml_diff>
--- a/main/parkslockup/parkslockup/user.xlsx
+++ b/main/parkslockup/parkslockup/user.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DX2"/>
+  <dimension ref="A1:DX4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,774 +423,1546 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.09485466778278351</v>
+        <v>-0.1382778733968735</v>
       </c>
       <c r="B1" t="n">
-        <v>0.06703618168830872</v>
+        <v>0.007945835590362549</v>
       </c>
       <c r="C1" t="n">
-        <v>0.02127917297184467</v>
+        <v>0.02911459654569626</v>
       </c>
       <c r="D1" t="n">
-        <v>-0.06376230716705322</v>
+        <v>-0.1102369502186775</v>
       </c>
       <c r="E1" t="n">
-        <v>-0.1364511251449585</v>
+        <v>-0.1382718831300735</v>
       </c>
       <c r="F1" t="n">
-        <v>-0.03535151109099388</v>
+        <v>-0.04958787187933922</v>
       </c>
       <c r="G1" t="n">
-        <v>-0.06387566775083542</v>
+        <v>-0.04737676680088043</v>
       </c>
       <c r="H1" t="n">
-        <v>-0.1082735806703568</v>
+        <v>-0.127418264746666</v>
       </c>
       <c r="I1" t="n">
-        <v>0.06820178776979446</v>
+        <v>0.1282702386379242</v>
       </c>
       <c r="J1" t="n">
-        <v>-0.08286596834659576</v>
+        <v>-0.1882466822862625</v>
       </c>
       <c r="K1" t="n">
-        <v>0.1804741621017456</v>
+        <v>0.1946576982736588</v>
       </c>
       <c r="L1" t="n">
-        <v>-0.1021347492933273</v>
+        <v>-0.01551858708262444</v>
       </c>
       <c r="M1" t="n">
-        <v>-0.1760626584291458</v>
+        <v>-0.1594134271144867</v>
       </c>
       <c r="N1" t="n">
-        <v>-0.03005245327949524</v>
+        <v>-0.09077514708042145</v>
       </c>
       <c r="O1" t="n">
-        <v>-0.05631003528833389</v>
+        <v>-0.03965058550238609</v>
       </c>
       <c r="P1" t="n">
-        <v>0.1911141872406006</v>
+        <v>0.1097557544708252</v>
       </c>
       <c r="Q1" t="n">
-        <v>-0.1526189744472504</v>
+        <v>-0.1154465228319168</v>
       </c>
       <c r="R1" t="n">
-        <v>-0.1408328413963318</v>
+        <v>-0.1321890652179718</v>
       </c>
       <c r="S1" t="n">
-        <v>-0.01263659074902534</v>
+        <v>-0.0604996457695961</v>
       </c>
       <c r="T1" t="n">
-        <v>-0.05120642483234406</v>
+        <v>-0.04805624485015869</v>
       </c>
       <c r="U1" t="n">
-        <v>0.1044452041387558</v>
+        <v>0.07097707688808441</v>
       </c>
       <c r="V1" t="n">
-        <v>0.03456606343388557</v>
+        <v>0.0174403078854084</v>
       </c>
       <c r="W1" t="n">
-        <v>-0.06797581911087036</v>
+        <v>0.03607260435819626</v>
       </c>
       <c r="X1" t="n">
-        <v>0.04859073460102081</v>
+        <v>0.04793576896190643</v>
       </c>
       <c r="Y1" t="n">
-        <v>-0.1289347559213638</v>
+        <v>-0.1198872700333595</v>
       </c>
       <c r="Z1" t="n">
-        <v>-0.2473560273647308</v>
+        <v>-0.3269570767879486</v>
       </c>
       <c r="AA1" t="n">
-        <v>-0.0812714621424675</v>
+        <v>-0.09239082038402557</v>
       </c>
       <c r="AB1" t="n">
-        <v>-0.04692735522985458</v>
+        <v>-0.06376546621322632</v>
       </c>
       <c r="AC1" t="n">
-        <v>0.04741709679365158</v>
+        <v>-0.08399349451065063</v>
       </c>
       <c r="AD1" t="n">
-        <v>-0.09473079442977905</v>
+        <v>-0.006296470761299133</v>
       </c>
       <c r="AE1" t="n">
-        <v>-0.04484916478395462</v>
+        <v>-0.02349697798490524</v>
       </c>
       <c r="AF1" t="n">
-        <v>0.08739297837018967</v>
+        <v>0.07426367700099945</v>
       </c>
       <c r="AG1" t="n">
-        <v>-0.1851689219474792</v>
+        <v>-0.1729133129119873</v>
       </c>
       <c r="AH1" t="n">
-        <v>-0.02788928896188736</v>
+        <v>-0.007488183677196503</v>
       </c>
       <c r="AI1" t="n">
-        <v>0.07642914354801178</v>
+        <v>-1.606345176696777e-05</v>
       </c>
       <c r="AJ1" t="n">
-        <v>0.1403133422136307</v>
+        <v>0.1516364961862564</v>
       </c>
       <c r="AK1" t="n">
-        <v>-0.03485668450593948</v>
+        <v>-0.02137750387191772</v>
       </c>
       <c r="AL1" t="n">
-        <v>-0.09182768315076828</v>
+        <v>-0.0494956448674202</v>
       </c>
       <c r="AM1" t="n">
-        <v>0.1478272676467896</v>
+        <v>0.1675834655761719</v>
       </c>
       <c r="AN1" t="n">
-        <v>0.002777041867375374</v>
+        <v>-0.01556148380041122</v>
       </c>
       <c r="AO1" t="n">
-        <v>-0.2373041808605194</v>
+        <v>-0.2267695069313049</v>
       </c>
       <c r="AP1" t="n">
-        <v>0.08068397641181946</v>
+        <v>0.01283149421215057</v>
       </c>
       <c r="AQ1" t="n">
-        <v>0.1014082208275795</v>
+        <v>0.06763863563537598</v>
       </c>
       <c r="AR1" t="n">
-        <v>0.2481510937213898</v>
+        <v>0.202142208814621</v>
       </c>
       <c r="AS1" t="n">
-        <v>0.1513766050338745</v>
+        <v>0.1471055299043655</v>
       </c>
       <c r="AT1" t="n">
-        <v>0.009458158165216446</v>
+        <v>-0.006245508790016174</v>
       </c>
       <c r="AU1" t="n">
-        <v>-0.01613818295300007</v>
+        <v>0.01341924257576466</v>
       </c>
       <c r="AV1" t="n">
-        <v>-0.1287010312080383</v>
+        <v>-0.1300828456878662</v>
       </c>
       <c r="AW1" t="n">
-        <v>0.1390102654695511</v>
+        <v>0.1269544363021851</v>
       </c>
       <c r="AX1" t="n">
-        <v>-0.1452124565839767</v>
+        <v>-0.1412402242422104</v>
       </c>
       <c r="AY1" t="n">
-        <v>0.03557280078530312</v>
+        <v>0.02571705542504787</v>
       </c>
       <c r="AZ1" t="n">
-        <v>0.1590018272399902</v>
+        <v>0.1479753851890564</v>
       </c>
       <c r="BA1" t="n">
-        <v>0.07602705061435699</v>
+        <v>0.0293671116232872</v>
       </c>
       <c r="BB1" t="n">
-        <v>0.09479926526546478</v>
+        <v>0.03299412131309509</v>
       </c>
       <c r="BC1" t="n">
-        <v>-0.001196503639221191</v>
+        <v>0.03129924833774567</v>
       </c>
       <c r="BD1" t="n">
-        <v>-0.1174946948885918</v>
+        <v>-0.09833343327045441</v>
       </c>
       <c r="BE1" t="n">
-        <v>0.04443830251693726</v>
+        <v>0.06239920854568481</v>
       </c>
       <c r="BF1" t="n">
-        <v>0.1309616565704346</v>
+        <v>0.1287360787391663</v>
       </c>
       <c r="BG1" t="n">
-        <v>-0.1108874455094337</v>
+        <v>-0.07938121259212494</v>
       </c>
       <c r="BH1" t="n">
-        <v>0.04732078313827515</v>
+        <v>-0.01887115836143494</v>
       </c>
       <c r="BI1" t="n">
-        <v>0.09111832827329636</v>
+        <v>0.03641126304864883</v>
       </c>
       <c r="BJ1" t="n">
-        <v>-0.05373813211917877</v>
+        <v>-0.09186064451932907</v>
       </c>
       <c r="BK1" t="n">
-        <v>0.0013433787971735</v>
+        <v>-0.05736681818962097</v>
       </c>
       <c r="BL1" t="n">
-        <v>-0.1251821517944336</v>
+        <v>-0.08586390316486359</v>
       </c>
       <c r="BM1" t="n">
-        <v>0.1769649684429169</v>
+        <v>0.2410064786672592</v>
       </c>
       <c r="BN1" t="n">
-        <v>0.04765579849481583</v>
+        <v>0.1228350102901459</v>
       </c>
       <c r="BO1" t="n">
-        <v>-0.1090299561619759</v>
+        <v>-0.1021574661135674</v>
       </c>
       <c r="BP1" t="n">
-        <v>-0.1749760061502457</v>
+        <v>-0.1827526986598969</v>
       </c>
       <c r="BQ1" t="n">
-        <v>0.1044353321194649</v>
+        <v>0.108033686876297</v>
       </c>
       <c r="BR1" t="n">
-        <v>-0.1287626624107361</v>
+        <v>-0.1393294632434845</v>
       </c>
       <c r="BS1" t="n">
-        <v>-0.1691557765007019</v>
+        <v>-0.1278384923934937</v>
       </c>
       <c r="BT1" t="n">
-        <v>0.05583389848470688</v>
+        <v>0.08007530122995377</v>
       </c>
       <c r="BU1" t="n">
-        <v>-0.1533361673355103</v>
+        <v>-0.1989483833312988</v>
       </c>
       <c r="BV1" t="n">
-        <v>-0.1494940221309662</v>
+        <v>-0.1833077520132065</v>
       </c>
       <c r="BW1" t="n">
-        <v>-0.2956796884536743</v>
+        <v>-0.2436062842607498</v>
       </c>
       <c r="BX1" t="n">
-        <v>0.01178117096424103</v>
+        <v>0.05002482235431671</v>
       </c>
       <c r="BY1" t="n">
-        <v>0.3653501272201538</v>
+        <v>0.3578956723213196</v>
       </c>
       <c r="BZ1" t="n">
-        <v>0.08812390267848969</v>
+        <v>0.125351145863533</v>
       </c>
       <c r="CA1" t="n">
-        <v>-0.2001336216926575</v>
+        <v>-0.1545947194099426</v>
       </c>
       <c r="CB1" t="n">
-        <v>0.09493726491928101</v>
+        <v>0.04842766374349594</v>
       </c>
       <c r="CC1" t="n">
-        <v>0.03564237058162689</v>
+        <v>-0.06581393629312515</v>
       </c>
       <c r="CD1" t="n">
-        <v>-0.01569591090083122</v>
+        <v>0.006299644708633423</v>
       </c>
       <c r="CE1" t="n">
-        <v>0.156116709113121</v>
+        <v>0.1572179198265076</v>
       </c>
       <c r="CF1" t="n">
-        <v>0.164734810590744</v>
+        <v>0.1557103246450424</v>
       </c>
       <c r="CG1" t="n">
-        <v>-0.008718930184841156</v>
+        <v>-0.01338757202029228</v>
       </c>
       <c r="CH1" t="n">
-        <v>0.02900025993585587</v>
+        <v>0.04317355901002884</v>
       </c>
       <c r="CI1" t="n">
-        <v>-0.02588922902941704</v>
+        <v>-0.07685787975788116</v>
       </c>
       <c r="CJ1" t="n">
-        <v>0.005427330732345581</v>
+        <v>0.04869863390922546</v>
       </c>
       <c r="CK1" t="n">
-        <v>0.3037063181400299</v>
+        <v>0.2434359639883041</v>
       </c>
       <c r="CL1" t="n">
-        <v>-0.04925555735826492</v>
+        <v>-0.05420609563589096</v>
       </c>
       <c r="CM1" t="n">
-        <v>-0.04288741573691368</v>
+        <v>-0.05577861145138741</v>
       </c>
       <c r="CN1" t="n">
-        <v>0.195686399936676</v>
+        <v>0.2162126898765564</v>
       </c>
       <c r="CO1" t="n">
-        <v>-0.01251985505223274</v>
+        <v>0.03697200119495392</v>
       </c>
       <c r="CP1" t="n">
-        <v>0.09499381482601166</v>
+        <v>0.1007369086146355</v>
       </c>
       <c r="CQ1" t="n">
-        <v>0.02258066646754742</v>
+        <v>0.01979565247893333</v>
       </c>
       <c r="CR1" t="n">
-        <v>0.01237185299396515</v>
+        <v>-0.03007097542285919</v>
       </c>
       <c r="CS1" t="n">
-        <v>-0.0174681544303894</v>
+        <v>-0.03968893736600876</v>
       </c>
       <c r="CT1" t="n">
-        <v>-0.004271131008863449</v>
+        <v>0.07312804460525513</v>
       </c>
       <c r="CU1" t="n">
-        <v>-0.1179265379905701</v>
+        <v>-0.1646886467933655</v>
       </c>
       <c r="CV1" t="n">
-        <v>-0.04873406887054443</v>
+        <v>0.02047304809093475</v>
       </c>
       <c r="CW1" t="n">
-        <v>0.04148821532726288</v>
+        <v>0.1049060672521591</v>
       </c>
       <c r="CX1" t="n">
-        <v>-0.09059341251850128</v>
+        <v>-0.02998721227049828</v>
       </c>
       <c r="CY1" t="n">
-        <v>-0.04875510931015015</v>
+        <v>-0.007661059498786926</v>
       </c>
       <c r="CZ1" t="n">
-        <v>0.1558375060558319</v>
+        <v>0.08773292601108551</v>
       </c>
       <c r="DA1" t="n">
-        <v>-0.1826533228158951</v>
+        <v>-0.1529325693845749</v>
       </c>
       <c r="DB1" t="n">
-        <v>0.1438359916210175</v>
+        <v>0.06628629565238953</v>
       </c>
       <c r="DC1" t="n">
-        <v>0.03894303739070892</v>
+        <v>-0.01514166593551636</v>
       </c>
       <c r="DD1" t="n">
-        <v>0.07702001184225082</v>
+        <v>0.005412917584180832</v>
       </c>
       <c r="DE1" t="n">
-        <v>0.001054786145687103</v>
+        <v>0.02755074948072433</v>
       </c>
       <c r="DF1" t="n">
-        <v>0.04926387965679169</v>
+        <v>-0.0345771312713623</v>
       </c>
       <c r="DG1" t="n">
-        <v>-0.1198687180876732</v>
+        <v>-0.114214725792408</v>
       </c>
       <c r="DH1" t="n">
-        <v>0.002067223191261292</v>
+        <v>-0.06649105250835419</v>
       </c>
       <c r="DI1" t="n">
-        <v>0.1401280462741852</v>
+        <v>0.10047797113657</v>
       </c>
       <c r="DJ1" t="n">
-        <v>-0.2177547216415405</v>
+        <v>-0.1966600120067596</v>
       </c>
       <c r="DK1" t="n">
-        <v>0.2690364420413971</v>
+        <v>0.2075463086366653</v>
       </c>
       <c r="DL1" t="n">
-        <v>0.1990942806005478</v>
+        <v>0.1737218797206879</v>
       </c>
       <c r="DM1" t="n">
-        <v>0.07974209636449814</v>
+        <v>0.1069902181625366</v>
       </c>
       <c r="DN1" t="n">
-        <v>0.03389789164066315</v>
+        <v>0.1458198428153992</v>
       </c>
       <c r="DO1" t="n">
-        <v>0.1731235533952713</v>
+        <v>0.1735578924417496</v>
       </c>
       <c r="DP1" t="n">
-        <v>0.03668829798698425</v>
+        <v>0.04669784009456635</v>
       </c>
       <c r="DQ1" t="n">
-        <v>0.03759229183197021</v>
+        <v>0.0268954262137413</v>
       </c>
       <c r="DR1" t="n">
-        <v>-0.02185090631246567</v>
+        <v>-0.0241331160068512</v>
       </c>
       <c r="DS1" t="n">
-        <v>-0.1961621344089508</v>
+        <v>-0.1943613439798355</v>
       </c>
       <c r="DT1" t="n">
-        <v>-0.05334164202213287</v>
+        <v>0.02617253176867962</v>
       </c>
       <c r="DU1" t="n">
-        <v>0.1355634182691574</v>
+        <v>0.1395968049764633</v>
       </c>
       <c r="DV1" t="n">
-        <v>-0.04713035374879837</v>
+        <v>0.003164835274219513</v>
       </c>
       <c r="DW1" t="n">
-        <v>0.05898511409759521</v>
+        <v>0.08271440863609314</v>
       </c>
       <c r="DX1" t="n">
-        <v>0.01923026889562607</v>
+        <v>-0.002608820796012878</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>-0.09485466778278351</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.06703618168830872</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.02127917297184467</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.06376230716705322</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.1364511251449585</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.03535151109099388</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-0.06387566775083542</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.1082735806703568</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.06820178776979446</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.08286596834659576</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.1804741621017456</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.1021347492933273</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.1760626584291458</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.03005245327949524</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.05631003528833389</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.1911141872406006</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.1526189744472504</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-0.1408328413963318</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-0.01263659074902534</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-0.05120642483234406</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1044452041387558</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.03456606343388557</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-0.06797581911087036</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.04859073460102081</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-0.1289347559213638</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-0.2473560273647308</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>-0.0812714621424675</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>-0.04692735522985458</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.04741709679365158</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-0.09473079442977905</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>-0.04484916478395462</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.08739297837018967</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>-0.1851689219474792</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>-0.02788928896188736</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.07642914354801178</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.1403133422136307</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>-0.03485668450593948</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>-0.09182768315076828</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.1478272676467896</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.002777041867375374</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>-0.2373041808605194</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.08068397641181946</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.1014082208275795</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.2481510937213898</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.1513766050338745</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.009458158165216446</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>-0.01613818295300007</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>-0.1287010312080383</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.1390102654695511</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>-0.1452124565839767</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.03557280078530312</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.1590018272399902</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.07602705061435699</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.09479926526546478</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>-0.001196503639221191</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>-0.1174946948885918</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.04443830251693726</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.1309616565704346</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>-0.1108874455094337</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.04732078313827515</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.09111832827329636</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>-0.05373813211917877</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.0013433787971735</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>-0.1251821517944336</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.1769649684429169</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.04765579849481583</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>-0.1090299561619759</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>-0.1749760061502457</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0.1044353321194649</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>-0.1287626624107361</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>-0.1691557765007019</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0.05583389848470688</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>-0.1533361673355103</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>-0.1494940221309662</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>-0.2956796884536743</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0.01178117096424103</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>0.3653501272201538</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0.08812390267848969</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>-0.2001336216926575</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.09493726491928101</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>0.03564237058162689</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>-0.01569591090083122</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>0.156116709113121</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0.164734810590744</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>-0.008718930184841156</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0.02900025993585587</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>-0.02588922902941704</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0.005427330732345581</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.3037063181400299</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>-0.04925555735826492</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>-0.04288741573691368</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0.195686399936676</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>-0.01251985505223274</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>0.09499381482601166</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0.02258066646754742</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0.01237185299396515</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>-0.0174681544303894</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>-0.004271131008863449</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>-0.1179265379905701</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>-0.04873406887054443</v>
+      </c>
+      <c r="CW2" t="n">
+        <v>0.04148821532726288</v>
+      </c>
+      <c r="CX2" t="n">
+        <v>-0.09059341251850128</v>
+      </c>
+      <c r="CY2" t="n">
+        <v>-0.04875510931015015</v>
+      </c>
+      <c r="CZ2" t="n">
+        <v>0.1558375060558319</v>
+      </c>
+      <c r="DA2" t="n">
+        <v>-0.1826533228158951</v>
+      </c>
+      <c r="DB2" t="n">
+        <v>0.1438359916210175</v>
+      </c>
+      <c r="DC2" t="n">
+        <v>0.03894303739070892</v>
+      </c>
+      <c r="DD2" t="n">
+        <v>0.07702001184225082</v>
+      </c>
+      <c r="DE2" t="n">
+        <v>0.001054786145687103</v>
+      </c>
+      <c r="DF2" t="n">
+        <v>0.04926387965679169</v>
+      </c>
+      <c r="DG2" t="n">
+        <v>-0.1198687180876732</v>
+      </c>
+      <c r="DH2" t="n">
+        <v>0.002067223191261292</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>0.1401280462741852</v>
+      </c>
+      <c r="DJ2" t="n">
+        <v>-0.2177547216415405</v>
+      </c>
+      <c r="DK2" t="n">
+        <v>0.2690364420413971</v>
+      </c>
+      <c r="DL2" t="n">
+        <v>0.1990942806005478</v>
+      </c>
+      <c r="DM2" t="n">
+        <v>0.07974209636449814</v>
+      </c>
+      <c r="DN2" t="n">
+        <v>0.03389789164066315</v>
+      </c>
+      <c r="DO2" t="n">
+        <v>0.1731235533952713</v>
+      </c>
+      <c r="DP2" t="n">
+        <v>0.03668829798698425</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>0.03759229183197021</v>
+      </c>
+      <c r="DR2" t="n">
+        <v>-0.02185090631246567</v>
+      </c>
+      <c r="DS2" t="n">
+        <v>-0.1961621344089508</v>
+      </c>
+      <c r="DT2" t="n">
+        <v>-0.05334164202213287</v>
+      </c>
+      <c r="DU2" t="n">
+        <v>0.1355634182691574</v>
+      </c>
+      <c r="DV2" t="n">
+        <v>-0.04713035374879837</v>
+      </c>
+      <c r="DW2" t="n">
+        <v>0.05898511409759521</v>
+      </c>
+      <c r="DX2" t="n">
+        <v>0.01923026889562607</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>-0.1730910390615463</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B3" t="n">
         <v>0.0468733087182045</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>0.02230261638760567</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D3" t="n">
         <v>-0.1236186027526855</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E3" t="n">
         <v>-0.1355118155479431</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F3" t="n">
         <v>-0.004758149385452271</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G3" t="n">
         <v>-0.04674947634339333</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H3" t="n">
         <v>-0.08549851924180984</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I3" t="n">
         <v>0.06096422672271729</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J3" t="n">
         <v>-0.1456707864999771</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K3" t="n">
         <v>0.1873953938484192</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L3" t="n">
         <v>-0.05990472063422203</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M3" t="n">
         <v>-0.2161078751087189</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N3" t="n">
         <v>-0.07083684206008911</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O3" t="n">
         <v>-0.05230434238910675</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P3" t="n">
         <v>0.1688528507947922</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q3" t="n">
         <v>-0.10996925085783</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R3" t="n">
         <v>-0.1554861068725586</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S3" t="n">
         <v>-0.06284290552139282</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T3" t="n">
         <v>0.01328445971012115</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U3" t="n">
         <v>0.09919625520706177</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V3" t="n">
         <v>0.06926415860652924</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W3" t="n">
         <v>-0.07293561846017838</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X3" t="n">
         <v>0.03993618488311768</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Y3" t="n">
         <v>-0.1648965626955032</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="Z3" t="n">
         <v>-0.2873676419258118</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA3" t="n">
         <v>-0.09258896857500076</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB3" t="n">
         <v>0.007343828678131104</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC3" t="n">
         <v>-0.08637028932571411</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AD3" t="n">
         <v>-0.08937422931194305</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AE3" t="n">
         <v>-0.0372329093515873</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF3" t="n">
         <v>0.05746649950742722</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG3" t="n">
         <v>-0.1870715022087097</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH3" t="n">
         <v>0.0144367516040802</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI3" t="n">
         <v>0.04682070761919022</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AJ3" t="n">
         <v>0.1388134360313416</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AK3" t="n">
         <v>0.01048935949802399</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AL3" t="n">
         <v>-0.01035474985837936</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AM3" t="n">
         <v>0.09950096905231476</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AN3" t="n">
         <v>0.04611104354262352</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AO3" t="n">
         <v>-0.2723390758037567</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AP3" t="n">
         <v>0.06730875372886658</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AQ3" t="n">
         <v>0.1117917224764824</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AR3" t="n">
         <v>0.2708423733711243</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AS3" t="n">
         <v>0.2074048519134521</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AT3" t="n">
         <v>-0.002255335450172424</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AU3" t="n">
         <v>-0.01857819408178329</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AV3" t="n">
         <v>-0.1428809612989426</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AW3" t="n">
         <v>0.1252310872077942</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AX3" t="n">
         <v>-0.2293906360864639</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AY3" t="n">
         <v>-0.04201679304242134</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="AZ3" t="n">
         <v>0.1312595307826996</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BA3" t="n">
         <v>0.03448783606290817</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BB3" t="n">
         <v>0.03538764268159866</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BC3" t="n">
         <v>-0.004816927015781403</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BD3" t="n">
         <v>-0.09243146330118179</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="BE3" t="n">
         <v>0.02554529905319214</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="BF3" t="n">
         <v>0.1159960031509399</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BG3" t="n">
         <v>-0.1160740330815315</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="BH3" t="n">
         <v>0.03537945449352264</v>
       </c>
-      <c r="BI2" t="n">
+      <c r="BI3" t="n">
         <v>0.06928659975528717</v>
       </c>
-      <c r="BJ2" t="n">
+      <c r="BJ3" t="n">
         <v>-0.1114377677440643</v>
       </c>
-      <c r="BK2" t="n">
+      <c r="BK3" t="n">
         <v>-0.08367887139320374</v>
       </c>
-      <c r="BL2" t="n">
+      <c r="BL3" t="n">
         <v>-0.1209922209382057</v>
       </c>
-      <c r="BM2" t="n">
+      <c r="BM3" t="n">
         <v>0.1632474362850189</v>
       </c>
-      <c r="BN2" t="n">
+      <c r="BN3" t="n">
         <v>0.03589450195431709</v>
       </c>
-      <c r="BO2" t="n">
+      <c r="BO3" t="n">
         <v>-0.1758359968662262</v>
       </c>
-      <c r="BP2" t="n">
+      <c r="BP3" t="n">
         <v>-0.2392930239439011</v>
       </c>
-      <c r="BQ2" t="n">
+      <c r="BQ3" t="n">
         <v>0.08649689704179764</v>
       </c>
-      <c r="BR2" t="n">
+      <c r="BR3" t="n">
         <v>-0.1891351044178009</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BS3" t="n">
         <v>-0.1356927454471588</v>
       </c>
-      <c r="BT2" t="n">
+      <c r="BT3" t="n">
         <v>0.1131480112671852</v>
       </c>
-      <c r="BU2" t="n">
+      <c r="BU3" t="n">
         <v>-0.1520384252071381</v>
       </c>
-      <c r="BV2" t="n">
+      <c r="BV3" t="n">
         <v>-0.2002529799938202</v>
       </c>
-      <c r="BW2" t="n">
+      <c r="BW3" t="n">
         <v>-0.3503864407539368</v>
       </c>
-      <c r="BX2" t="n">
+      <c r="BX3" t="n">
         <v>0.03609529137611389</v>
       </c>
-      <c r="BY2" t="n">
+      <c r="BY3" t="n">
         <v>0.3386359214782715</v>
       </c>
-      <c r="BZ2" t="n">
+      <c r="BZ3" t="n">
         <v>0.1422533094882965</v>
       </c>
-      <c r="CA2" t="n">
+      <c r="CA3" t="n">
         <v>-0.1987703293561935</v>
       </c>
-      <c r="CB2" t="n">
+      <c r="CB3" t="n">
         <v>0.08287635445594788</v>
       </c>
-      <c r="CC2" t="n">
+      <c r="CC3" t="n">
         <v>0.008811849169433117</v>
       </c>
-      <c r="CD2" t="n">
+      <c r="CD3" t="n">
         <v>0.04027725756168365</v>
       </c>
-      <c r="CE2" t="n">
+      <c r="CE3" t="n">
         <v>0.1274399161338806</v>
       </c>
-      <c r="CF2" t="n">
+      <c r="CF3" t="n">
         <v>0.1737797409296036</v>
       </c>
-      <c r="CG2" t="n">
+      <c r="CG3" t="n">
         <v>0.007274281233549118</v>
       </c>
-      <c r="CH2" t="n">
+      <c r="CH3" t="n">
         <v>0.06602674722671509</v>
       </c>
-      <c r="CI2" t="n">
+      <c r="CI3" t="n">
         <v>-0.08098559081554413</v>
       </c>
-      <c r="CJ2" t="n">
+      <c r="CJ3" t="n">
         <v>0.06098867952823639</v>
       </c>
-      <c r="CK2" t="n">
+      <c r="CK3" t="n">
         <v>0.2891929149627686</v>
       </c>
-      <c r="CL2" t="n">
+      <c r="CL3" t="n">
         <v>-0.04164474457502365</v>
       </c>
-      <c r="CM2" t="n">
+      <c r="CM3" t="n">
         <v>-0.008886042982339859</v>
       </c>
-      <c r="CN2" t="n">
+      <c r="CN3" t="n">
         <v>0.2377078533172607</v>
       </c>
-      <c r="CO2" t="n">
+      <c r="CO3" t="n">
         <v>0.02674798667430878</v>
       </c>
-      <c r="CP2" t="n">
+      <c r="CP3" t="n">
         <v>0.1161438524723053</v>
       </c>
-      <c r="CQ2" t="n">
+      <c r="CQ3" t="n">
         <v>0.01022475212812424</v>
       </c>
-      <c r="CR2" t="n">
+      <c r="CR3" t="n">
         <v>0.06723983585834503</v>
       </c>
-      <c r="CS2" t="n">
+      <c r="CS3" t="n">
         <v>-0.04888508468866348</v>
       </c>
-      <c r="CT2" t="n">
+      <c r="CT3" t="n">
         <v>-0.02901731431484222</v>
       </c>
-      <c r="CU2" t="n">
+      <c r="CU3" t="n">
         <v>-0.1517019271850586</v>
       </c>
-      <c r="CV2" t="n">
+      <c r="CV3" t="n">
         <v>0.003211945295333862</v>
       </c>
-      <c r="CW2" t="n">
+      <c r="CW3" t="n">
         <v>0.04904887825250626</v>
       </c>
-      <c r="CX2" t="n">
+      <c r="CX3" t="n">
         <v>-0.03636002540588379</v>
       </c>
-      <c r="CY2" t="n">
+      <c r="CY3" t="n">
         <v>0.001870393753051758</v>
       </c>
-      <c r="CZ2" t="n">
+      <c r="CZ3" t="n">
         <v>0.1718954145908356</v>
       </c>
-      <c r="DA2" t="n">
+      <c r="DA3" t="n">
         <v>-0.1269590258598328</v>
       </c>
-      <c r="DB2" t="n">
+      <c r="DB3" t="n">
         <v>0.1904156804084778</v>
       </c>
-      <c r="DC2" t="n">
+      <c r="DC3" t="n">
         <v>-0.0403340682387352</v>
       </c>
-      <c r="DD2" t="n">
+      <c r="DD3" t="n">
         <v>0.03302508220076561</v>
       </c>
-      <c r="DE2" t="n">
+      <c r="DE3" t="n">
         <v>-0.03621438145637512</v>
       </c>
-      <c r="DF2" t="n">
+      <c r="DF3" t="n">
         <v>-0.03502778708934784</v>
       </c>
-      <c r="DG2" t="n">
+      <c r="DG3" t="n">
         <v>-0.07337862998247147</v>
       </c>
-      <c r="DH2" t="n">
+      <c r="DH3" t="n">
         <v>0.005858689546585083</v>
       </c>
-      <c r="DI2" t="n">
+      <c r="DI3" t="n">
         <v>0.08885832130908966</v>
       </c>
-      <c r="DJ2" t="n">
+      <c r="DJ3" t="n">
         <v>-0.2003527730703354</v>
       </c>
-      <c r="DK2" t="n">
+      <c r="DK3" t="n">
         <v>0.1659952402114868</v>
       </c>
-      <c r="DL2" t="n">
+      <c r="DL3" t="n">
         <v>0.2087558507919312</v>
       </c>
-      <c r="DM2" t="n">
+      <c r="DM3" t="n">
         <v>0.08905559778213501</v>
       </c>
-      <c r="DN2" t="n">
+      <c r="DN3" t="n">
         <v>0.03161385282874107</v>
       </c>
-      <c r="DO2" t="n">
+      <c r="DO3" t="n">
         <v>0.1914173662662506</v>
       </c>
-      <c r="DP2" t="n">
+      <c r="DP3" t="n">
         <v>-0.002605810761451721</v>
       </c>
-      <c r="DQ2" t="n">
+      <c r="DQ3" t="n">
         <v>-0.005448907613754272</v>
       </c>
-      <c r="DR2" t="n">
+      <c r="DR3" t="n">
         <v>0.03450989723205566</v>
       </c>
-      <c r="DS2" t="n">
+      <c r="DS3" t="n">
         <v>-0.2104713171720505</v>
       </c>
-      <c r="DT2" t="n">
+      <c r="DT3" t="n">
         <v>-0.03083633072674274</v>
       </c>
-      <c r="DU2" t="n">
+      <c r="DU3" t="n">
         <v>0.09877301007509232</v>
       </c>
-      <c r="DV2" t="n">
+      <c r="DV3" t="n">
         <v>-0.1010307371616364</v>
       </c>
-      <c r="DW2" t="n">
+      <c r="DW3" t="n">
         <v>0.09877075254917145</v>
       </c>
-      <c r="DX2" t="n">
+      <c r="DX3" t="n">
         <v>-0.04287730902433395</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-0.1265500485897064</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.052773118019104</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.03113424405455589</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.02856689319014549</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.1167944073677063</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.05147958546876907</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.02914068102836609</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.0967031717300415</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1138124391436577</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.131234884262085</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.1872152984142303</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.01861658319830894</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.2146996408700943</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.03237511590123177</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.03487748652696609</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.1559838950634003</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.103147029876709</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.1523146331310272</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.1058259084820747</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-0.01321998238563538</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.06601934134960175</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.01493392884731293</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.03503106907010078</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.02962133288383484</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>-0.1363294422626495</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>-0.3141153752803802</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>-0.08970241993665695</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>-0.04383113235235214</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-0.04840630665421486</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.01288542151451111</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>-0.06733457744121552</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.07180865108966827</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>-0.1543737500905991</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>-0.0268133357167244</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.03853920847177505</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.1541158109903336</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>-0.03069610893726349</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>-0.05951587855815887</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.1880277395248413</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>-0.002621769905090332</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>-0.2270280420780182</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.004334092140197754</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.05371517688035965</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.2508932650089264</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0.1678507924079895</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>-0.007513541728258133</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.03020026162266731</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>-0.0976569652557373</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>0.09889533370733261</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>-0.2260507941246033</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.01609216257929802</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>0.1301730126142502</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.05221081525087357</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.09152357280254364</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>-0.02669250220060349</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>-0.07871381938457489</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>0.1052104830741882</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>0.1244325488805771</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>-0.1209468320012093</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>-0.05309294164180756</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.09676355123519897</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>-0.1505133509635925</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>-0.09572853147983551</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>-0.07758187502622604</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.2299387902021408</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>0.1138094663619995</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>-0.1087143570184708</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>-0.181447446346283</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>0.06344742327928543</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>-0.1682620495557785</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>-0.1249397769570351</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>0.03562940284609795</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>-0.167438417673111</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>-0.1518743932247162</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>-0.304784744977951</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>0.02694137394428253</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>0.3864977359771729</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>0.1446642726659775</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>-0.1520258486270905</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>0.08836635947227478</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>-0.04046059027314186</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>0.03495679795742035</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>0.1301746070384979</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>0.1207738593220711</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>-0.04280385002493858</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0.06248047947883606</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>-0.1344617754220963</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>0.05777309834957123</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>0.245211586356163</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>-0.08524768799543381</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>-0.02847550250589848</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>0.1869578510522842</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>0.05987383425235748</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>0.1164320111274719</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>0.04716560244560242</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>0.01386433839797974</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>-0.02070973813533783</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>0.01532096788287163</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>-0.1451727598905563</v>
+      </c>
+      <c r="CV4" t="n">
+        <v>0.03620017319917679</v>
+      </c>
+      <c r="CW4" t="n">
+        <v>0.09348283708095551</v>
+      </c>
+      <c r="CX4" t="n">
+        <v>-0.004446474835276604</v>
+      </c>
+      <c r="CY4" t="n">
+        <v>0.002868473529815674</v>
+      </c>
+      <c r="CZ4" t="n">
+        <v>0.06505899876356125</v>
+      </c>
+      <c r="DA4" t="n">
+        <v>-0.1446656286716461</v>
+      </c>
+      <c r="DB4" t="n">
+        <v>0.1354619413614273</v>
+      </c>
+      <c r="DC4" t="n">
+        <v>-0.02313166856765747</v>
+      </c>
+      <c r="DD4" t="n">
+        <v>0.03633891046047211</v>
+      </c>
+      <c r="DE4" t="n">
+        <v>0.04738517850637436</v>
+      </c>
+      <c r="DF4" t="n">
+        <v>-0.06536491215229034</v>
+      </c>
+      <c r="DG4" t="n">
+        <v>-0.1013645827770233</v>
+      </c>
+      <c r="DH4" t="n">
+        <v>-0.05722665786743164</v>
+      </c>
+      <c r="DI4" t="n">
+        <v>0.0991760790348053</v>
+      </c>
+      <c r="DJ4" t="n">
+        <v>-0.1798270493745804</v>
+      </c>
+      <c r="DK4" t="n">
+        <v>0.1431812345981598</v>
+      </c>
+      <c r="DL4" t="n">
+        <v>0.1779062151908875</v>
+      </c>
+      <c r="DM4" t="n">
+        <v>0.0675027146935463</v>
+      </c>
+      <c r="DN4" t="n">
+        <v>0.1118984892964363</v>
+      </c>
+      <c r="DO4" t="n">
+        <v>0.1660496443510056</v>
+      </c>
+      <c r="DP4" t="n">
+        <v>0.04290303587913513</v>
+      </c>
+      <c r="DQ4" t="n">
+        <v>-0.0223298966884613</v>
+      </c>
+      <c r="DR4" t="n">
+        <v>0.02490139007568359</v>
+      </c>
+      <c r="DS4" t="n">
+        <v>-0.2426488995552063</v>
+      </c>
+      <c r="DT4" t="n">
+        <v>-0.01144071202725172</v>
+      </c>
+      <c r="DU4" t="n">
+        <v>0.1421199440956116</v>
+      </c>
+      <c r="DV4" t="n">
+        <v>-0.004106044769287109</v>
+      </c>
+      <c r="DW4" t="n">
+        <v>0.08463555574417114</v>
+      </c>
+      <c r="DX4" t="n">
+        <v>0.01743845269083977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADD] face recognition only using xlsx file
</commit_message>
<xml_diff>
--- a/main/parkslockup/parkslockup/user.xlsx
+++ b/main/parkslockup/parkslockup/user.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DX4"/>
+  <dimension ref="A1:DY5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,1546 +422,1957 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ChoiMinJay</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
         <v>-0.1382778733968735</v>
       </c>
-      <c r="B1" t="n">
+      <c r="C1" t="n">
         <v>0.007945835590362549</v>
       </c>
-      <c r="C1" t="n">
+      <c r="D1" t="n">
         <v>0.02911459654569626</v>
       </c>
-      <c r="D1" t="n">
+      <c r="E1" t="n">
         <v>-0.1102369502186775</v>
       </c>
-      <c r="E1" t="n">
+      <c r="F1" t="n">
         <v>-0.1382718831300735</v>
       </c>
-      <c r="F1" t="n">
+      <c r="G1" t="n">
         <v>-0.04958787187933922</v>
       </c>
-      <c r="G1" t="n">
+      <c r="H1" t="n">
         <v>-0.04737676680088043</v>
       </c>
-      <c r="H1" t="n">
+      <c r="I1" t="n">
         <v>-0.127418264746666</v>
       </c>
-      <c r="I1" t="n">
+      <c r="J1" t="n">
         <v>0.1282702386379242</v>
       </c>
-      <c r="J1" t="n">
+      <c r="K1" t="n">
         <v>-0.1882466822862625</v>
       </c>
-      <c r="K1" t="n">
+      <c r="L1" t="n">
         <v>0.1946576982736588</v>
       </c>
-      <c r="L1" t="n">
+      <c r="M1" t="n">
         <v>-0.01551858708262444</v>
       </c>
-      <c r="M1" t="n">
+      <c r="N1" t="n">
         <v>-0.1594134271144867</v>
       </c>
-      <c r="N1" t="n">
+      <c r="O1" t="n">
         <v>-0.09077514708042145</v>
       </c>
-      <c r="O1" t="n">
+      <c r="P1" t="n">
         <v>-0.03965058550238609</v>
       </c>
-      <c r="P1" t="n">
+      <c r="Q1" t="n">
         <v>0.1097557544708252</v>
       </c>
-      <c r="Q1" t="n">
+      <c r="R1" t="n">
         <v>-0.1154465228319168</v>
       </c>
-      <c r="R1" t="n">
+      <c r="S1" t="n">
         <v>-0.1321890652179718</v>
       </c>
-      <c r="S1" t="n">
+      <c r="T1" t="n">
         <v>-0.0604996457695961</v>
       </c>
-      <c r="T1" t="n">
+      <c r="U1" t="n">
         <v>-0.04805624485015869</v>
       </c>
-      <c r="U1" t="n">
+      <c r="V1" t="n">
         <v>0.07097707688808441</v>
       </c>
-      <c r="V1" t="n">
+      <c r="W1" t="n">
         <v>0.0174403078854084</v>
       </c>
-      <c r="W1" t="n">
+      <c r="X1" t="n">
         <v>0.03607260435819626</v>
       </c>
-      <c r="X1" t="n">
+      <c r="Y1" t="n">
         <v>0.04793576896190643</v>
       </c>
-      <c r="Y1" t="n">
+      <c r="Z1" t="n">
         <v>-0.1198872700333595</v>
       </c>
-      <c r="Z1" t="n">
+      <c r="AA1" t="n">
         <v>-0.3269570767879486</v>
       </c>
-      <c r="AA1" t="n">
+      <c r="AB1" t="n">
         <v>-0.09239082038402557</v>
       </c>
-      <c r="AB1" t="n">
+      <c r="AC1" t="n">
         <v>-0.06376546621322632</v>
       </c>
-      <c r="AC1" t="n">
+      <c r="AD1" t="n">
         <v>-0.08399349451065063</v>
       </c>
-      <c r="AD1" t="n">
+      <c r="AE1" t="n">
         <v>-0.006296470761299133</v>
       </c>
-      <c r="AE1" t="n">
+      <c r="AF1" t="n">
         <v>-0.02349697798490524</v>
       </c>
-      <c r="AF1" t="n">
+      <c r="AG1" t="n">
         <v>0.07426367700099945</v>
       </c>
-      <c r="AG1" t="n">
+      <c r="AH1" t="n">
         <v>-0.1729133129119873</v>
       </c>
-      <c r="AH1" t="n">
+      <c r="AI1" t="n">
         <v>-0.007488183677196503</v>
       </c>
-      <c r="AI1" t="n">
+      <c r="AJ1" t="n">
         <v>-1.606345176696777e-05</v>
       </c>
-      <c r="AJ1" t="n">
+      <c r="AK1" t="n">
         <v>0.1516364961862564</v>
       </c>
-      <c r="AK1" t="n">
+      <c r="AL1" t="n">
         <v>-0.02137750387191772</v>
       </c>
-      <c r="AL1" t="n">
+      <c r="AM1" t="n">
         <v>-0.0494956448674202</v>
       </c>
-      <c r="AM1" t="n">
+      <c r="AN1" t="n">
         <v>0.1675834655761719</v>
       </c>
-      <c r="AN1" t="n">
+      <c r="AO1" t="n">
         <v>-0.01556148380041122</v>
       </c>
-      <c r="AO1" t="n">
+      <c r="AP1" t="n">
         <v>-0.2267695069313049</v>
       </c>
-      <c r="AP1" t="n">
+      <c r="AQ1" t="n">
         <v>0.01283149421215057</v>
       </c>
-      <c r="AQ1" t="n">
+      <c r="AR1" t="n">
         <v>0.06763863563537598</v>
       </c>
-      <c r="AR1" t="n">
+      <c r="AS1" t="n">
         <v>0.202142208814621</v>
       </c>
-      <c r="AS1" t="n">
+      <c r="AT1" t="n">
         <v>0.1471055299043655</v>
       </c>
-      <c r="AT1" t="n">
+      <c r="AU1" t="n">
         <v>-0.006245508790016174</v>
       </c>
-      <c r="AU1" t="n">
+      <c r="AV1" t="n">
         <v>0.01341924257576466</v>
       </c>
-      <c r="AV1" t="n">
+      <c r="AW1" t="n">
         <v>-0.1300828456878662</v>
       </c>
-      <c r="AW1" t="n">
+      <c r="AX1" t="n">
         <v>0.1269544363021851</v>
       </c>
-      <c r="AX1" t="n">
+      <c r="AY1" t="n">
         <v>-0.1412402242422104</v>
       </c>
-      <c r="AY1" t="n">
+      <c r="AZ1" t="n">
         <v>0.02571705542504787</v>
       </c>
-      <c r="AZ1" t="n">
+      <c r="BA1" t="n">
         <v>0.1479753851890564</v>
       </c>
-      <c r="BA1" t="n">
+      <c r="BB1" t="n">
         <v>0.0293671116232872</v>
       </c>
-      <c r="BB1" t="n">
+      <c r="BC1" t="n">
         <v>0.03299412131309509</v>
       </c>
-      <c r="BC1" t="n">
+      <c r="BD1" t="n">
         <v>0.03129924833774567</v>
       </c>
-      <c r="BD1" t="n">
+      <c r="BE1" t="n">
         <v>-0.09833343327045441</v>
       </c>
-      <c r="BE1" t="n">
+      <c r="BF1" t="n">
         <v>0.06239920854568481</v>
       </c>
-      <c r="BF1" t="n">
+      <c r="BG1" t="n">
         <v>0.1287360787391663</v>
       </c>
-      <c r="BG1" t="n">
+      <c r="BH1" t="n">
         <v>-0.07938121259212494</v>
       </c>
-      <c r="BH1" t="n">
+      <c r="BI1" t="n">
         <v>-0.01887115836143494</v>
       </c>
-      <c r="BI1" t="n">
+      <c r="BJ1" t="n">
         <v>0.03641126304864883</v>
       </c>
-      <c r="BJ1" t="n">
+      <c r="BK1" t="n">
         <v>-0.09186064451932907</v>
       </c>
-      <c r="BK1" t="n">
+      <c r="BL1" t="n">
         <v>-0.05736681818962097</v>
       </c>
-      <c r="BL1" t="n">
+      <c r="BM1" t="n">
         <v>-0.08586390316486359</v>
       </c>
-      <c r="BM1" t="n">
+      <c r="BN1" t="n">
         <v>0.2410064786672592</v>
       </c>
-      <c r="BN1" t="n">
+      <c r="BO1" t="n">
         <v>0.1228350102901459</v>
       </c>
-      <c r="BO1" t="n">
+      <c r="BP1" t="n">
         <v>-0.1021574661135674</v>
       </c>
-      <c r="BP1" t="n">
+      <c r="BQ1" t="n">
         <v>-0.1827526986598969</v>
       </c>
-      <c r="BQ1" t="n">
+      <c r="BR1" t="n">
         <v>0.108033686876297</v>
       </c>
-      <c r="BR1" t="n">
+      <c r="BS1" t="n">
         <v>-0.1393294632434845</v>
       </c>
-      <c r="BS1" t="n">
+      <c r="BT1" t="n">
         <v>-0.1278384923934937</v>
       </c>
-      <c r="BT1" t="n">
+      <c r="BU1" t="n">
         <v>0.08007530122995377</v>
       </c>
-      <c r="BU1" t="n">
+      <c r="BV1" t="n">
         <v>-0.1989483833312988</v>
       </c>
-      <c r="BV1" t="n">
+      <c r="BW1" t="n">
         <v>-0.1833077520132065</v>
       </c>
-      <c r="BW1" t="n">
+      <c r="BX1" t="n">
         <v>-0.2436062842607498</v>
       </c>
-      <c r="BX1" t="n">
+      <c r="BY1" t="n">
         <v>0.05002482235431671</v>
       </c>
-      <c r="BY1" t="n">
+      <c r="BZ1" t="n">
         <v>0.3578956723213196</v>
       </c>
-      <c r="BZ1" t="n">
+      <c r="CA1" t="n">
         <v>0.125351145863533</v>
       </c>
-      <c r="CA1" t="n">
+      <c r="CB1" t="n">
         <v>-0.1545947194099426</v>
       </c>
-      <c r="CB1" t="n">
+      <c r="CC1" t="n">
         <v>0.04842766374349594</v>
       </c>
-      <c r="CC1" t="n">
+      <c r="CD1" t="n">
         <v>-0.06581393629312515</v>
       </c>
-      <c r="CD1" t="n">
+      <c r="CE1" t="n">
         <v>0.006299644708633423</v>
       </c>
-      <c r="CE1" t="n">
+      <c r="CF1" t="n">
         <v>0.1572179198265076</v>
       </c>
-      <c r="CF1" t="n">
+      <c r="CG1" t="n">
         <v>0.1557103246450424</v>
       </c>
-      <c r="CG1" t="n">
+      <c r="CH1" t="n">
         <v>-0.01338757202029228</v>
       </c>
-      <c r="CH1" t="n">
+      <c r="CI1" t="n">
         <v>0.04317355901002884</v>
       </c>
-      <c r="CI1" t="n">
+      <c r="CJ1" t="n">
         <v>-0.07685787975788116</v>
       </c>
-      <c r="CJ1" t="n">
+      <c r="CK1" t="n">
         <v>0.04869863390922546</v>
       </c>
-      <c r="CK1" t="n">
+      <c r="CL1" t="n">
         <v>0.2434359639883041</v>
       </c>
-      <c r="CL1" t="n">
+      <c r="CM1" t="n">
         <v>-0.05420609563589096</v>
       </c>
-      <c r="CM1" t="n">
+      <c r="CN1" t="n">
         <v>-0.05577861145138741</v>
       </c>
-      <c r="CN1" t="n">
+      <c r="CO1" t="n">
         <v>0.2162126898765564</v>
       </c>
-      <c r="CO1" t="n">
+      <c r="CP1" t="n">
         <v>0.03697200119495392</v>
       </c>
-      <c r="CP1" t="n">
+      <c r="CQ1" t="n">
         <v>0.1007369086146355</v>
       </c>
-      <c r="CQ1" t="n">
+      <c r="CR1" t="n">
         <v>0.01979565247893333</v>
       </c>
-      <c r="CR1" t="n">
+      <c r="CS1" t="n">
         <v>-0.03007097542285919</v>
       </c>
-      <c r="CS1" t="n">
+      <c r="CT1" t="n">
         <v>-0.03968893736600876</v>
       </c>
-      <c r="CT1" t="n">
+      <c r="CU1" t="n">
         <v>0.07312804460525513</v>
       </c>
-      <c r="CU1" t="n">
+      <c r="CV1" t="n">
         <v>-0.1646886467933655</v>
       </c>
-      <c r="CV1" t="n">
+      <c r="CW1" t="n">
         <v>0.02047304809093475</v>
       </c>
-      <c r="CW1" t="n">
+      <c r="CX1" t="n">
         <v>0.1049060672521591</v>
       </c>
-      <c r="CX1" t="n">
+      <c r="CY1" t="n">
         <v>-0.02998721227049828</v>
       </c>
-      <c r="CY1" t="n">
+      <c r="CZ1" t="n">
         <v>-0.007661059498786926</v>
       </c>
-      <c r="CZ1" t="n">
+      <c r="DA1" t="n">
         <v>0.08773292601108551</v>
       </c>
-      <c r="DA1" t="n">
+      <c r="DB1" t="n">
         <v>-0.1529325693845749</v>
       </c>
-      <c r="DB1" t="n">
+      <c r="DC1" t="n">
         <v>0.06628629565238953</v>
       </c>
-      <c r="DC1" t="n">
+      <c r="DD1" t="n">
         <v>-0.01514166593551636</v>
       </c>
-      <c r="DD1" t="n">
+      <c r="DE1" t="n">
         <v>0.005412917584180832</v>
       </c>
-      <c r="DE1" t="n">
+      <c r="DF1" t="n">
         <v>0.02755074948072433</v>
       </c>
-      <c r="DF1" t="n">
+      <c r="DG1" t="n">
         <v>-0.0345771312713623</v>
       </c>
-      <c r="DG1" t="n">
+      <c r="DH1" t="n">
         <v>-0.114214725792408</v>
       </c>
-      <c r="DH1" t="n">
+      <c r="DI1" t="n">
         <v>-0.06649105250835419</v>
       </c>
-      <c r="DI1" t="n">
+      <c r="DJ1" t="n">
         <v>0.10047797113657</v>
       </c>
-      <c r="DJ1" t="n">
+      <c r="DK1" t="n">
         <v>-0.1966600120067596</v>
       </c>
-      <c r="DK1" t="n">
+      <c r="DL1" t="n">
         <v>0.2075463086366653</v>
       </c>
-      <c r="DL1" t="n">
+      <c r="DM1" t="n">
         <v>0.1737218797206879</v>
       </c>
-      <c r="DM1" t="n">
+      <c r="DN1" t="n">
         <v>0.1069902181625366</v>
       </c>
-      <c r="DN1" t="n">
+      <c r="DO1" t="n">
         <v>0.1458198428153992</v>
       </c>
-      <c r="DO1" t="n">
+      <c r="DP1" t="n">
         <v>0.1735578924417496</v>
       </c>
-      <c r="DP1" t="n">
+      <c r="DQ1" t="n">
         <v>0.04669784009456635</v>
       </c>
-      <c r="DQ1" t="n">
+      <c r="DR1" t="n">
         <v>0.0268954262137413</v>
       </c>
-      <c r="DR1" t="n">
+      <c r="DS1" t="n">
         <v>-0.0241331160068512</v>
       </c>
-      <c r="DS1" t="n">
+      <c r="DT1" t="n">
         <v>-0.1943613439798355</v>
       </c>
-      <c r="DT1" t="n">
+      <c r="DU1" t="n">
         <v>0.02617253176867962</v>
       </c>
-      <c r="DU1" t="n">
+      <c r="DV1" t="n">
         <v>0.1395968049764633</v>
       </c>
-      <c r="DV1" t="n">
+      <c r="DW1" t="n">
         <v>0.003164835274219513</v>
       </c>
-      <c r="DW1" t="n">
+      <c r="DX1" t="n">
         <v>0.08271440863609314</v>
       </c>
-      <c r="DX1" t="n">
+      <c r="DY1" t="n">
         <v>-0.002608820796012878</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>-0.09485466778278351</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hansangbin</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.06703618168830872</v>
+        <v>-0.02872360497713089</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02127917297184467</v>
+        <v>0.004404798150062561</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.06376230716705322</v>
+        <v>0.008789112791419029</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1364511251449585</v>
+        <v>-0.03327016904950142</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.03535151109099388</v>
+        <v>-0.1423420608043671</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.06387566775083542</v>
+        <v>-0.06323243677616119</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.1082735806703568</v>
+        <v>-0.07461117208003998</v>
       </c>
       <c r="I2" t="n">
-        <v>0.06820178776979446</v>
+        <v>-0.1119554564356804</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.08286596834659576</v>
+        <v>0.09407861530780792</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1804741621017456</v>
+        <v>-0.1013293340802193</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.1021347492933273</v>
+        <v>0.2370283901691437</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.1760626584291458</v>
+        <v>-0.06358348578214645</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.03005245327949524</v>
+        <v>-0.1869285702705383</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.05631003528833389</v>
+        <v>-0.08540138602256775</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1911141872406006</v>
+        <v>-0.08300720155239105</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.1526189744472504</v>
+        <v>0.1701486110687256</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.1408328413963318</v>
+        <v>-0.1092158854007721</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.01263659074902534</v>
+        <v>-0.09970957040786743</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.05120642483234406</v>
+        <v>-0.06600780040025711</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1044452041387558</v>
+        <v>0.03019768744707108</v>
       </c>
       <c r="V2" t="n">
-        <v>0.03456606343388557</v>
+        <v>0.09886746108531952</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.06797581911087036</v>
+        <v>-0.004406342748552561</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04859073460102081</v>
+        <v>-0.02574936673045158</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.1289347559213638</v>
+        <v>0.02524749934673309</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.2473560273647308</v>
+        <v>-0.06007522344589233</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.0812714621424675</v>
+        <v>-0.2943963408470154</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.04692735522985458</v>
+        <v>-0.07807746529579163</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.04741709679365158</v>
+        <v>-0.06800507754087448</v>
       </c>
       <c r="AD2" t="n">
-        <v>-0.09473079442977905</v>
+        <v>-0.01156849041581154</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.04484916478395462</v>
+        <v>-0.1011481285095215</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.08739297837018967</v>
+        <v>-0.06500376015901566</v>
       </c>
       <c r="AG2" t="n">
-        <v>-0.1851689219474792</v>
+        <v>0.0176439955830574</v>
       </c>
       <c r="AH2" t="n">
-        <v>-0.02788928896188736</v>
+        <v>-0.2013198435306549</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.07642914354801178</v>
+        <v>-0.09448647499084473</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.1403133422136307</v>
+        <v>0.06149572879076004</v>
       </c>
       <c r="AK2" t="n">
-        <v>-0.03485668450593948</v>
+        <v>0.06174866855144501</v>
       </c>
       <c r="AL2" t="n">
-        <v>-0.09182768315076828</v>
+        <v>-0.03200182318687439</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.1478272676467896</v>
+        <v>-0.06830893456935883</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.002777041867375374</v>
+        <v>0.1291183233261108</v>
       </c>
       <c r="AO2" t="n">
-        <v>-0.2373041808605194</v>
+        <v>0.007487052120268345</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.08068397641181946</v>
+        <v>-0.2524104714393616</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.1014082208275795</v>
+        <v>0.04138267040252686</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.2481510937213898</v>
+        <v>0.02328458428382874</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.1513766050338745</v>
+        <v>0.1979120969772339</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.009458158165216446</v>
+        <v>0.1816067397594452</v>
       </c>
       <c r="AU2" t="n">
-        <v>-0.01613818295300007</v>
+        <v>0.04092879965901375</v>
       </c>
       <c r="AV2" t="n">
-        <v>-0.1287010312080383</v>
+        <v>0.02378034591674805</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.1390102654695511</v>
+        <v>-0.1838584840297699</v>
       </c>
       <c r="AX2" t="n">
-        <v>-0.1452124565839767</v>
+        <v>0.1759032607078552</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.03557280078530312</v>
+        <v>-0.165059894323349</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0.1590018272399902</v>
+        <v>0.06786153465509415</v>
       </c>
       <c r="BA2" t="n">
-        <v>0.07602705061435699</v>
+        <v>0.07740604132413864</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.09479926526546478</v>
+        <v>0.1847184896469116</v>
       </c>
       <c r="BC2" t="n">
-        <v>-0.001196503639221191</v>
+        <v>0.002637751400470734</v>
       </c>
       <c r="BD2" t="n">
-        <v>-0.1174946948885918</v>
+        <v>-0.02480719983577728</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.04443830251693726</v>
+        <v>-0.1027178093791008</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.1309616565704346</v>
+        <v>0.02060222625732422</v>
       </c>
       <c r="BG2" t="n">
-        <v>-0.1108874455094337</v>
+        <v>0.1786413192749023</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.04732078313827515</v>
+        <v>-0.181621327996254</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.09111832827329636</v>
+        <v>0.05773743242025375</v>
       </c>
       <c r="BJ2" t="n">
-        <v>-0.05373813211917877</v>
+        <v>0.1271576434373856</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.0013433787971735</v>
+        <v>-0.08171959221363068</v>
       </c>
       <c r="BL2" t="n">
-        <v>-0.1251821517944336</v>
+        <v>-0.08280429244041443</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.1769649684429169</v>
+        <v>-0.08819226920604706</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.04765579849481583</v>
+        <v>0.1928559690713882</v>
       </c>
       <c r="BO2" t="n">
-        <v>-0.1090299561619759</v>
+        <v>0.06757354736328125</v>
       </c>
       <c r="BP2" t="n">
-        <v>-0.1749760061502457</v>
+        <v>-0.1320914030075073</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.1044353321194649</v>
+        <v>-0.1956077218055725</v>
       </c>
       <c r="BR2" t="n">
-        <v>-0.1287626624107361</v>
+        <v>0.1412539184093475</v>
       </c>
       <c r="BS2" t="n">
-        <v>-0.1691557765007019</v>
+        <v>-0.1302027404308319</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.05583389848470688</v>
+        <v>-0.08783823996782303</v>
       </c>
       <c r="BU2" t="n">
-        <v>-0.1533361673355103</v>
+        <v>0.06112609803676605</v>
       </c>
       <c r="BV2" t="n">
-        <v>-0.1494940221309662</v>
+        <v>-0.1397953629493713</v>
       </c>
       <c r="BW2" t="n">
-        <v>-0.2956796884536743</v>
+        <v>-0.2204681485891342</v>
       </c>
       <c r="BX2" t="n">
-        <v>0.01178117096424103</v>
+        <v>-0.3110555708408356</v>
       </c>
       <c r="BY2" t="n">
-        <v>0.3653501272201538</v>
+        <v>0.02850474417209625</v>
       </c>
       <c r="BZ2" t="n">
-        <v>0.08812390267848969</v>
+        <v>0.3883723616600037</v>
       </c>
       <c r="CA2" t="n">
-        <v>-0.2001336216926575</v>
+        <v>0.1011334508657455</v>
       </c>
       <c r="CB2" t="n">
-        <v>0.09493726491928101</v>
+        <v>-0.23698590695858</v>
       </c>
       <c r="CC2" t="n">
-        <v>0.03564237058162689</v>
+        <v>0.002632088959217072</v>
       </c>
       <c r="CD2" t="n">
-        <v>-0.01569591090083122</v>
+        <v>-0.0370212085545063</v>
       </c>
       <c r="CE2" t="n">
-        <v>0.156116709113121</v>
+        <v>0.06517493724822998</v>
       </c>
       <c r="CF2" t="n">
-        <v>0.164734810590744</v>
+        <v>0.116234190762043</v>
       </c>
       <c r="CG2" t="n">
-        <v>-0.008718930184841156</v>
+        <v>0.1446985900402069</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.02900025993585587</v>
+        <v>0.02624869719147682</v>
       </c>
       <c r="CI2" t="n">
-        <v>-0.02588922902941704</v>
+        <v>0.01273453235626221</v>
       </c>
       <c r="CJ2" t="n">
-        <v>0.005427330732345581</v>
+        <v>-0.08973339200019836</v>
       </c>
       <c r="CK2" t="n">
-        <v>0.3037063181400299</v>
+        <v>-0.009245574474334717</v>
       </c>
       <c r="CL2" t="n">
-        <v>-0.04925555735826492</v>
+        <v>0.2187029868364334</v>
       </c>
       <c r="CM2" t="n">
-        <v>-0.04288741573691368</v>
+        <v>-0.1093813180923462</v>
       </c>
       <c r="CN2" t="n">
-        <v>0.195686399936676</v>
+        <v>-0.04895563051104546</v>
       </c>
       <c r="CO2" t="n">
-        <v>-0.01251985505223274</v>
+        <v>0.1951891183853149</v>
       </c>
       <c r="CP2" t="n">
-        <v>0.09499381482601166</v>
+        <v>-0.03105670213699341</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.02258066646754742</v>
+        <v>0.07600542902946472</v>
       </c>
       <c r="CR2" t="n">
-        <v>0.01237185299396515</v>
+        <v>-0.007472587283700705</v>
       </c>
       <c r="CS2" t="n">
-        <v>-0.0174681544303894</v>
+        <v>0.007342204451560974</v>
       </c>
       <c r="CT2" t="n">
-        <v>-0.004271131008863449</v>
+        <v>-0.06933575868606567</v>
       </c>
       <c r="CU2" t="n">
-        <v>-0.1179265379905701</v>
+        <v>0.04102551937103271</v>
       </c>
       <c r="CV2" t="n">
-        <v>-0.04873406887054443</v>
+        <v>-0.1176632568240166</v>
       </c>
       <c r="CW2" t="n">
-        <v>0.04148821532726288</v>
+        <v>-0.04516885429620743</v>
       </c>
       <c r="CX2" t="n">
-        <v>-0.09059341251850128</v>
+        <v>0.05391570180654526</v>
       </c>
       <c r="CY2" t="n">
-        <v>-0.04875510931015015</v>
+        <v>0.009970164857804775</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.1558375060558319</v>
+        <v>0.008529365062713623</v>
       </c>
       <c r="DA2" t="n">
-        <v>-0.1826533228158951</v>
+        <v>0.1165604591369629</v>
       </c>
       <c r="DB2" t="n">
-        <v>0.1438359916210175</v>
+        <v>-0.09540696442127228</v>
       </c>
       <c r="DC2" t="n">
-        <v>0.03894303739070892</v>
+        <v>0.1236195936799049</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.07702001184225082</v>
+        <v>-0.05242388695478439</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.001054786145687103</v>
+        <v>0.04939109459519386</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.04926387965679169</v>
+        <v>0.04890945553779602</v>
       </c>
       <c r="DG2" t="n">
-        <v>-0.1198687180876732</v>
+        <v>-0.08045114576816559</v>
       </c>
       <c r="DH2" t="n">
-        <v>0.002067223191261292</v>
+        <v>-0.08226922154426575</v>
       </c>
       <c r="DI2" t="n">
-        <v>0.1401280462741852</v>
+        <v>-0.07440656423568726</v>
       </c>
       <c r="DJ2" t="n">
-        <v>-0.2177547216415405</v>
+        <v>0.1043661832809448</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.2690364420413971</v>
+        <v>-0.1846476644277573</v>
       </c>
       <c r="DL2" t="n">
-        <v>0.1990942806005478</v>
+        <v>0.2098342627286911</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.07974209636449814</v>
+        <v>0.1261157244443893</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.03389789164066315</v>
+        <v>0.1281517744064331</v>
       </c>
       <c r="DO2" t="n">
-        <v>0.1731235533952713</v>
+        <v>0.07763391733169556</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.03668829798698425</v>
+        <v>0.1212636157870293</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.03759229183197021</v>
+        <v>0.04057663679122925</v>
       </c>
       <c r="DR2" t="n">
-        <v>-0.02185090631246567</v>
+        <v>0.04651129245758057</v>
       </c>
       <c r="DS2" t="n">
-        <v>-0.1961621344089508</v>
+        <v>-0.03749749809503555</v>
       </c>
       <c r="DT2" t="n">
-        <v>-0.05334164202213287</v>
+        <v>-0.2639769911766052</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.1355634182691574</v>
+        <v>-0.009984535165131092</v>
       </c>
       <c r="DV2" t="n">
-        <v>-0.04713035374879837</v>
+        <v>0.1216832399368286</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.05898511409759521</v>
+        <v>-0.03771978616714478</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.01923026889562607</v>
+        <v>0.09510312974452972</v>
+      </c>
+      <c r="DY2" t="n">
+        <v>-0.04387351125478745</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>-0.1730910390615463</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ParkByoungkwan</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0468733087182045</v>
+        <v>-0.09485466778278351</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02230261638760567</v>
+        <v>0.06703618168830872</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1236186027526855</v>
+        <v>0.02127917297184467</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1355118155479431</v>
+        <v>-0.06376230716705322</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.004758149385452271</v>
+        <v>-0.1364511251449585</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.04674947634339333</v>
+        <v>-0.03535151109099388</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.08549851924180984</v>
+        <v>-0.06387566775083542</v>
       </c>
       <c r="I3" t="n">
-        <v>0.06096422672271729</v>
+        <v>-0.1082735806703568</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.1456707864999771</v>
+        <v>0.06820178776979446</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1873953938484192</v>
+        <v>-0.08286596834659576</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.05990472063422203</v>
+        <v>0.1804741621017456</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.2161078751087189</v>
+        <v>-0.1021347492933273</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.07083684206008911</v>
+        <v>-0.1760626584291458</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.05230434238910675</v>
+        <v>-0.03005245327949524</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1688528507947922</v>
+        <v>-0.05631003528833389</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.10996925085783</v>
+        <v>0.1911141872406006</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.1554861068725586</v>
+        <v>-0.1526189744472504</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.06284290552139282</v>
+        <v>-0.1408328413963318</v>
       </c>
       <c r="T3" t="n">
-        <v>0.01328445971012115</v>
+        <v>-0.01263659074902534</v>
       </c>
       <c r="U3" t="n">
-        <v>0.09919625520706177</v>
+        <v>-0.05120642483234406</v>
       </c>
       <c r="V3" t="n">
-        <v>0.06926415860652924</v>
+        <v>0.1044452041387558</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.07293561846017838</v>
+        <v>0.03456606343388557</v>
       </c>
       <c r="X3" t="n">
-        <v>0.03993618488311768</v>
+        <v>-0.06797581911087036</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.1648965626955032</v>
+        <v>0.04859073460102081</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.2873676419258118</v>
+        <v>-0.1289347559213638</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.09258896857500076</v>
+        <v>-0.2473560273647308</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.007343828678131104</v>
+        <v>-0.0812714621424675</v>
       </c>
       <c r="AC3" t="n">
-        <v>-0.08637028932571411</v>
+        <v>-0.04692735522985458</v>
       </c>
       <c r="AD3" t="n">
-        <v>-0.08937422931194305</v>
+        <v>0.04741709679365158</v>
       </c>
       <c r="AE3" t="n">
-        <v>-0.0372329093515873</v>
+        <v>-0.09473079442977905</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.05746649950742722</v>
+        <v>-0.04484916478395462</v>
       </c>
       <c r="AG3" t="n">
-        <v>-0.1870715022087097</v>
+        <v>0.08739297837018967</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.0144367516040802</v>
+        <v>-0.1851689219474792</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.04682070761919022</v>
+        <v>-0.02788928896188736</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.1388134360313416</v>
+        <v>0.07642914354801178</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.01048935949802399</v>
+        <v>0.1403133422136307</v>
       </c>
       <c r="AL3" t="n">
-        <v>-0.01035474985837936</v>
+        <v>-0.03485668450593948</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.09950096905231476</v>
+        <v>-0.09182768315076828</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.04611104354262352</v>
+        <v>0.1478272676467896</v>
       </c>
       <c r="AO3" t="n">
-        <v>-0.2723390758037567</v>
+        <v>0.002777041867375374</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.06730875372886658</v>
+        <v>-0.2373041808605194</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.1117917224764824</v>
+        <v>0.08068397641181946</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.2708423733711243</v>
+        <v>0.1014082208275795</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.2074048519134521</v>
+        <v>0.2481510937213898</v>
       </c>
       <c r="AT3" t="n">
-        <v>-0.002255335450172424</v>
+        <v>0.1513766050338745</v>
       </c>
       <c r="AU3" t="n">
-        <v>-0.01857819408178329</v>
+        <v>0.009458158165216446</v>
       </c>
       <c r="AV3" t="n">
-        <v>-0.1428809612989426</v>
+        <v>-0.01613818295300007</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.1252310872077942</v>
+        <v>-0.1287010312080383</v>
       </c>
       <c r="AX3" t="n">
-        <v>-0.2293906360864639</v>
+        <v>0.1390102654695511</v>
       </c>
       <c r="AY3" t="n">
-        <v>-0.04201679304242134</v>
+        <v>-0.1452124565839767</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.1312595307826996</v>
+        <v>0.03557280078530312</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.03448783606290817</v>
+        <v>0.1590018272399902</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.03538764268159866</v>
+        <v>0.07602705061435699</v>
       </c>
       <c r="BC3" t="n">
-        <v>-0.004816927015781403</v>
+        <v>0.09479926526546478</v>
       </c>
       <c r="BD3" t="n">
-        <v>-0.09243146330118179</v>
+        <v>-0.001196503639221191</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.02554529905319214</v>
+        <v>-0.1174946948885918</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.1159960031509399</v>
+        <v>0.04443830251693726</v>
       </c>
       <c r="BG3" t="n">
-        <v>-0.1160740330815315</v>
+        <v>0.1309616565704346</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.03537945449352264</v>
+        <v>-0.1108874455094337</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.06928659975528717</v>
+        <v>0.04732078313827515</v>
       </c>
       <c r="BJ3" t="n">
-        <v>-0.1114377677440643</v>
+        <v>0.09111832827329636</v>
       </c>
       <c r="BK3" t="n">
-        <v>-0.08367887139320374</v>
+        <v>-0.05373813211917877</v>
       </c>
       <c r="BL3" t="n">
-        <v>-0.1209922209382057</v>
+        <v>0.0013433787971735</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.1632474362850189</v>
+        <v>-0.1251821517944336</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.03589450195431709</v>
+        <v>0.1769649684429169</v>
       </c>
       <c r="BO3" t="n">
-        <v>-0.1758359968662262</v>
+        <v>0.04765579849481583</v>
       </c>
       <c r="BP3" t="n">
-        <v>-0.2392930239439011</v>
+        <v>-0.1090299561619759</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.08649689704179764</v>
+        <v>-0.1749760061502457</v>
       </c>
       <c r="BR3" t="n">
-        <v>-0.1891351044178009</v>
+        <v>0.1044353321194649</v>
       </c>
       <c r="BS3" t="n">
-        <v>-0.1356927454471588</v>
+        <v>-0.1287626624107361</v>
       </c>
       <c r="BT3" t="n">
-        <v>0.1131480112671852</v>
+        <v>-0.1691557765007019</v>
       </c>
       <c r="BU3" t="n">
-        <v>-0.1520384252071381</v>
+        <v>0.05583389848470688</v>
       </c>
       <c r="BV3" t="n">
-        <v>-0.2002529799938202</v>
+        <v>-0.1533361673355103</v>
       </c>
       <c r="BW3" t="n">
-        <v>-0.3503864407539368</v>
+        <v>-0.1494940221309662</v>
       </c>
       <c r="BX3" t="n">
-        <v>0.03609529137611389</v>
+        <v>-0.2956796884536743</v>
       </c>
       <c r="BY3" t="n">
-        <v>0.3386359214782715</v>
+        <v>0.01178117096424103</v>
       </c>
       <c r="BZ3" t="n">
-        <v>0.1422533094882965</v>
+        <v>0.3653501272201538</v>
       </c>
       <c r="CA3" t="n">
-        <v>-0.1987703293561935</v>
+        <v>0.08812390267848969</v>
       </c>
       <c r="CB3" t="n">
-        <v>0.08287635445594788</v>
+        <v>-0.2001336216926575</v>
       </c>
       <c r="CC3" t="n">
-        <v>0.008811849169433117</v>
+        <v>0.09493726491928101</v>
       </c>
       <c r="CD3" t="n">
-        <v>0.04027725756168365</v>
+        <v>0.03564237058162689</v>
       </c>
       <c r="CE3" t="n">
-        <v>0.1274399161338806</v>
+        <v>-0.01569591090083122</v>
       </c>
       <c r="CF3" t="n">
-        <v>0.1737797409296036</v>
+        <v>0.156116709113121</v>
       </c>
       <c r="CG3" t="n">
-        <v>0.007274281233549118</v>
+        <v>0.164734810590744</v>
       </c>
       <c r="CH3" t="n">
-        <v>0.06602674722671509</v>
+        <v>-0.008718930184841156</v>
       </c>
       <c r="CI3" t="n">
-        <v>-0.08098559081554413</v>
+        <v>0.02900025993585587</v>
       </c>
       <c r="CJ3" t="n">
-        <v>0.06098867952823639</v>
+        <v>-0.02588922902941704</v>
       </c>
       <c r="CK3" t="n">
-        <v>0.2891929149627686</v>
+        <v>0.005427330732345581</v>
       </c>
       <c r="CL3" t="n">
-        <v>-0.04164474457502365</v>
+        <v>0.3037063181400299</v>
       </c>
       <c r="CM3" t="n">
-        <v>-0.008886042982339859</v>
+        <v>-0.04925555735826492</v>
       </c>
       <c r="CN3" t="n">
-        <v>0.2377078533172607</v>
+        <v>-0.04288741573691368</v>
       </c>
       <c r="CO3" t="n">
-        <v>0.02674798667430878</v>
+        <v>0.195686399936676</v>
       </c>
       <c r="CP3" t="n">
-        <v>0.1161438524723053</v>
+        <v>-0.01251985505223274</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.01022475212812424</v>
+        <v>0.09499381482601166</v>
       </c>
       <c r="CR3" t="n">
-        <v>0.06723983585834503</v>
+        <v>0.02258066646754742</v>
       </c>
       <c r="CS3" t="n">
-        <v>-0.04888508468866348</v>
+        <v>0.01237185299396515</v>
       </c>
       <c r="CT3" t="n">
-        <v>-0.02901731431484222</v>
+        <v>-0.0174681544303894</v>
       </c>
       <c r="CU3" t="n">
-        <v>-0.1517019271850586</v>
+        <v>-0.004271131008863449</v>
       </c>
       <c r="CV3" t="n">
-        <v>0.003211945295333862</v>
+        <v>-0.1179265379905701</v>
       </c>
       <c r="CW3" t="n">
-        <v>0.04904887825250626</v>
+        <v>-0.04873406887054443</v>
       </c>
       <c r="CX3" t="n">
-        <v>-0.03636002540588379</v>
+        <v>0.04148821532726288</v>
       </c>
       <c r="CY3" t="n">
-        <v>0.001870393753051758</v>
+        <v>-0.09059341251850128</v>
       </c>
       <c r="CZ3" t="n">
-        <v>0.1718954145908356</v>
+        <v>-0.04875510931015015</v>
       </c>
       <c r="DA3" t="n">
-        <v>-0.1269590258598328</v>
+        <v>0.1558375060558319</v>
       </c>
       <c r="DB3" t="n">
-        <v>0.1904156804084778</v>
+        <v>-0.1826533228158951</v>
       </c>
       <c r="DC3" t="n">
-        <v>-0.0403340682387352</v>
+        <v>0.1438359916210175</v>
       </c>
       <c r="DD3" t="n">
-        <v>0.03302508220076561</v>
+        <v>0.03894303739070892</v>
       </c>
       <c r="DE3" t="n">
-        <v>-0.03621438145637512</v>
+        <v>0.07702001184225082</v>
       </c>
       <c r="DF3" t="n">
-        <v>-0.03502778708934784</v>
+        <v>0.001054786145687103</v>
       </c>
       <c r="DG3" t="n">
-        <v>-0.07337862998247147</v>
+        <v>0.04926387965679169</v>
       </c>
       <c r="DH3" t="n">
-        <v>0.005858689546585083</v>
+        <v>-0.1198687180876732</v>
       </c>
       <c r="DI3" t="n">
-        <v>0.08885832130908966</v>
+        <v>0.002067223191261292</v>
       </c>
       <c r="DJ3" t="n">
-        <v>-0.2003527730703354</v>
+        <v>0.1401280462741852</v>
       </c>
       <c r="DK3" t="n">
-        <v>0.1659952402114868</v>
+        <v>-0.2177547216415405</v>
       </c>
       <c r="DL3" t="n">
-        <v>0.2087558507919312</v>
+        <v>0.2690364420413971</v>
       </c>
       <c r="DM3" t="n">
-        <v>0.08905559778213501</v>
+        <v>0.1990942806005478</v>
       </c>
       <c r="DN3" t="n">
-        <v>0.03161385282874107</v>
+        <v>0.07974209636449814</v>
       </c>
       <c r="DO3" t="n">
-        <v>0.1914173662662506</v>
+        <v>0.03389789164066315</v>
       </c>
       <c r="DP3" t="n">
-        <v>-0.002605810761451721</v>
+        <v>0.1731235533952713</v>
       </c>
       <c r="DQ3" t="n">
-        <v>-0.005448907613754272</v>
+        <v>0.03668829798698425</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.03450989723205566</v>
+        <v>0.03759229183197021</v>
       </c>
       <c r="DS3" t="n">
-        <v>-0.2104713171720505</v>
+        <v>-0.02185090631246567</v>
       </c>
       <c r="DT3" t="n">
-        <v>-0.03083633072674274</v>
+        <v>-0.1961621344089508</v>
       </c>
       <c r="DU3" t="n">
-        <v>0.09877301007509232</v>
+        <v>-0.05334164202213287</v>
       </c>
       <c r="DV3" t="n">
-        <v>-0.1010307371616364</v>
+        <v>0.1355634182691574</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.09877075254917145</v>
+        <v>-0.04713035374879837</v>
       </c>
       <c r="DX3" t="n">
-        <v>-0.04287730902433395</v>
+        <v>0.05898511409759521</v>
+      </c>
+      <c r="DY3" t="n">
+        <v>0.01923026889562607</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kijun</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.1730910390615463</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0468733087182045</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.02230261638760567</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.1236186027526855</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.1355118155479431</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.004758149385452271</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.04674947634339333</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.08549851924180984</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.06096422672271729</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.1456707864999771</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.1873953938484192</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.05990472063422203</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.2161078751087189</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.07083684206008911</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.05230434238910675</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.1688528507947922</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.10996925085783</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.1554861068725586</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-0.06284290552139282</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.01328445971012115</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.09919625520706177</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.06926415860652924</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-0.07293561846017838</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.03993618488311768</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>-0.1648965626955032</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>-0.2873676419258118</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>-0.09258896857500076</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.007343828678131104</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>-0.08637028932571411</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>-0.08937422931194305</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>-0.0372329093515873</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.05746649950742722</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>-0.1870715022087097</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.0144367516040802</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.04682070761919022</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.1388134360313416</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.01048935949802399</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>-0.01035474985837936</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.09950096905231476</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.04611104354262352</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>-0.2723390758037567</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.06730875372886658</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.1117917224764824</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0.2708423733711243</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.2074048519134521</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>-0.002255335450172424</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>-0.01857819408178329</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>-0.1428809612989426</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.1252310872077942</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>-0.2293906360864639</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>-0.04201679304242134</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.1312595307826996</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.03448783606290817</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0.03538764268159866</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>-0.004816927015781403</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>-0.09243146330118179</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>0.02554529905319214</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>0.1159960031509399</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>-0.1160740330815315</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.03537945449352264</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.06928659975528717</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>-0.1114377677440643</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>-0.08367887139320374</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>-0.1209922209382057</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>0.1632474362850189</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0.03589450195431709</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>-0.1758359968662262</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>-0.2392930239439011</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>0.08649689704179764</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>-0.1891351044178009</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>-0.1356927454471588</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>0.1131480112671852</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>-0.1520384252071381</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>-0.2002529799938202</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>-0.3503864407539368</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>0.03609529137611389</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>0.3386359214782715</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>0.1422533094882965</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>-0.1987703293561935</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>0.08287635445594788</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>0.008811849169433117</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>0.04027725756168365</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>0.1274399161338806</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>0.1737797409296036</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0.007274281233549118</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>0.06602674722671509</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>-0.08098559081554413</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>0.06098867952823639</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>0.2891929149627686</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>-0.04164474457502365</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>-0.008886042982339859</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>0.2377078533172607</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>0.02674798667430878</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>0.1161438524723053</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>0.01022475212812424</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>0.06723983585834503</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>-0.04888508468866348</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>-0.02901731431484222</v>
+      </c>
+      <c r="CV4" t="n">
+        <v>-0.1517019271850586</v>
+      </c>
+      <c r="CW4" t="n">
+        <v>0.003211945295333862</v>
+      </c>
+      <c r="CX4" t="n">
+        <v>0.04904887825250626</v>
+      </c>
+      <c r="CY4" t="n">
+        <v>-0.03636002540588379</v>
+      </c>
+      <c r="CZ4" t="n">
+        <v>0.001870393753051758</v>
+      </c>
+      <c r="DA4" t="n">
+        <v>0.1718954145908356</v>
+      </c>
+      <c r="DB4" t="n">
+        <v>-0.1269590258598328</v>
+      </c>
+      <c r="DC4" t="n">
+        <v>0.1904156804084778</v>
+      </c>
+      <c r="DD4" t="n">
+        <v>-0.0403340682387352</v>
+      </c>
+      <c r="DE4" t="n">
+        <v>0.03302508220076561</v>
+      </c>
+      <c r="DF4" t="n">
+        <v>-0.03621438145637512</v>
+      </c>
+      <c r="DG4" t="n">
+        <v>-0.03502778708934784</v>
+      </c>
+      <c r="DH4" t="n">
+        <v>-0.07337862998247147</v>
+      </c>
+      <c r="DI4" t="n">
+        <v>0.005858689546585083</v>
+      </c>
+      <c r="DJ4" t="n">
+        <v>0.08885832130908966</v>
+      </c>
+      <c r="DK4" t="n">
+        <v>-0.2003527730703354</v>
+      </c>
+      <c r="DL4" t="n">
+        <v>0.1659952402114868</v>
+      </c>
+      <c r="DM4" t="n">
+        <v>0.2087558507919312</v>
+      </c>
+      <c r="DN4" t="n">
+        <v>0.08905559778213501</v>
+      </c>
+      <c r="DO4" t="n">
+        <v>0.03161385282874107</v>
+      </c>
+      <c r="DP4" t="n">
+        <v>0.1914173662662506</v>
+      </c>
+      <c r="DQ4" t="n">
+        <v>-0.002605810761451721</v>
+      </c>
+      <c r="DR4" t="n">
+        <v>-0.005448907613754272</v>
+      </c>
+      <c r="DS4" t="n">
+        <v>0.03450989723205566</v>
+      </c>
+      <c r="DT4" t="n">
+        <v>-0.2104713171720505</v>
+      </c>
+      <c r="DU4" t="n">
+        <v>-0.03083633072674274</v>
+      </c>
+      <c r="DV4" t="n">
+        <v>0.09877301007509232</v>
+      </c>
+      <c r="DW4" t="n">
+        <v>-0.1010307371616364</v>
+      </c>
+      <c r="DX4" t="n">
+        <v>0.09877075254917145</v>
+      </c>
+      <c r="DY4" t="n">
+        <v>-0.04287730902433395</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Parksunghan</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>-0.1265500485897064</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C5" t="n">
         <v>0.052773118019104</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D5" t="n">
         <v>0.03113424405455589</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E5" t="n">
         <v>-0.02856689319014549</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F5" t="n">
         <v>-0.1167944073677063</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G5" t="n">
         <v>-0.05147958546876907</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H5" t="n">
         <v>-0.02914068102836609</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I5" t="n">
         <v>-0.0967031717300415</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J5" t="n">
         <v>0.1138124391436577</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K5" t="n">
         <v>-0.131234884262085</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L5" t="n">
         <v>0.1872152984142303</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M5" t="n">
         <v>-0.01861658319830894</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N5" t="n">
         <v>-0.2146996408700943</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O5" t="n">
         <v>-0.03237511590123177</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P5" t="n">
         <v>-0.03487748652696609</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q5" t="n">
         <v>0.1559838950634003</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R5" t="n">
         <v>-0.103147029876709</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S5" t="n">
         <v>-0.1523146331310272</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T5" t="n">
         <v>-0.1058259084820747</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U5" t="n">
         <v>-0.01321998238563538</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V5" t="n">
         <v>0.06601934134960175</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W5" t="n">
         <v>0.01493392884731293</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X5" t="n">
         <v>0.03503106907010078</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y5" t="n">
         <v>0.02962133288383484</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Z5" t="n">
         <v>-0.1363294422626495</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AA5" t="n">
         <v>-0.3141153752803802</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB5" t="n">
         <v>-0.08970241993665695</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC5" t="n">
         <v>-0.04383113235235214</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD5" t="n">
         <v>-0.04840630665421486</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AE5" t="n">
         <v>0.01288542151451111</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AF5" t="n">
         <v>-0.06733457744121552</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AG5" t="n">
         <v>0.07180865108966827</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AH5" t="n">
         <v>-0.1543737500905991</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AI5" t="n">
         <v>-0.0268133357167244</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AJ5" t="n">
         <v>0.03853920847177505</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AK5" t="n">
         <v>0.1541158109903336</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AL5" t="n">
         <v>-0.03069610893726349</v>
       </c>
-      <c r="AL4" t="n">
+      <c r="AM5" t="n">
         <v>-0.05951587855815887</v>
       </c>
-      <c r="AM4" t="n">
+      <c r="AN5" t="n">
         <v>0.1880277395248413</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AO5" t="n">
         <v>-0.002621769905090332</v>
       </c>
-      <c r="AO4" t="n">
+      <c r="AP5" t="n">
         <v>-0.2270280420780182</v>
       </c>
-      <c r="AP4" t="n">
+      <c r="AQ5" t="n">
         <v>0.004334092140197754</v>
       </c>
-      <c r="AQ4" t="n">
+      <c r="AR5" t="n">
         <v>0.05371517688035965</v>
       </c>
-      <c r="AR4" t="n">
+      <c r="AS5" t="n">
         <v>0.2508932650089264</v>
       </c>
-      <c r="AS4" t="n">
+      <c r="AT5" t="n">
         <v>0.1678507924079895</v>
       </c>
-      <c r="AT4" t="n">
+      <c r="AU5" t="n">
         <v>-0.007513541728258133</v>
       </c>
-      <c r="AU4" t="n">
+      <c r="AV5" t="n">
         <v>0.03020026162266731</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="AW5" t="n">
         <v>-0.0976569652557373</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="AX5" t="n">
         <v>0.09889533370733261</v>
       </c>
-      <c r="AX4" t="n">
+      <c r="AY5" t="n">
         <v>-0.2260507941246033</v>
       </c>
-      <c r="AY4" t="n">
+      <c r="AZ5" t="n">
         <v>0.01609216257929802</v>
       </c>
-      <c r="AZ4" t="n">
+      <c r="BA5" t="n">
         <v>0.1301730126142502</v>
       </c>
-      <c r="BA4" t="n">
+      <c r="BB5" t="n">
         <v>0.05221081525087357</v>
       </c>
-      <c r="BB4" t="n">
+      <c r="BC5" t="n">
         <v>0.09152357280254364</v>
       </c>
-      <c r="BC4" t="n">
+      <c r="BD5" t="n">
         <v>-0.02669250220060349</v>
       </c>
-      <c r="BD4" t="n">
+      <c r="BE5" t="n">
         <v>-0.07871381938457489</v>
       </c>
-      <c r="BE4" t="n">
+      <c r="BF5" t="n">
         <v>0.1052104830741882</v>
       </c>
-      <c r="BF4" t="n">
+      <c r="BG5" t="n">
         <v>0.1244325488805771</v>
       </c>
-      <c r="BG4" t="n">
+      <c r="BH5" t="n">
         <v>-0.1209468320012093</v>
       </c>
-      <c r="BH4" t="n">
+      <c r="BI5" t="n">
         <v>-0.05309294164180756</v>
       </c>
-      <c r="BI4" t="n">
+      <c r="BJ5" t="n">
         <v>0.09676355123519897</v>
       </c>
-      <c r="BJ4" t="n">
+      <c r="BK5" t="n">
         <v>-0.1505133509635925</v>
       </c>
-      <c r="BK4" t="n">
+      <c r="BL5" t="n">
         <v>-0.09572853147983551</v>
       </c>
-      <c r="BL4" t="n">
+      <c r="BM5" t="n">
         <v>-0.07758187502622604</v>
       </c>
-      <c r="BM4" t="n">
+      <c r="BN5" t="n">
         <v>0.2299387902021408</v>
       </c>
-      <c r="BN4" t="n">
+      <c r="BO5" t="n">
         <v>0.1138094663619995</v>
       </c>
-      <c r="BO4" t="n">
+      <c r="BP5" t="n">
         <v>-0.1087143570184708</v>
       </c>
-      <c r="BP4" t="n">
+      <c r="BQ5" t="n">
         <v>-0.181447446346283</v>
       </c>
-      <c r="BQ4" t="n">
+      <c r="BR5" t="n">
         <v>0.06344742327928543</v>
       </c>
-      <c r="BR4" t="n">
+      <c r="BS5" t="n">
         <v>-0.1682620495557785</v>
       </c>
-      <c r="BS4" t="n">
+      <c r="BT5" t="n">
         <v>-0.1249397769570351</v>
       </c>
-      <c r="BT4" t="n">
+      <c r="BU5" t="n">
         <v>0.03562940284609795</v>
       </c>
-      <c r="BU4" t="n">
+      <c r="BV5" t="n">
         <v>-0.167438417673111</v>
       </c>
-      <c r="BV4" t="n">
+      <c r="BW5" t="n">
         <v>-0.1518743932247162</v>
       </c>
-      <c r="BW4" t="n">
+      <c r="BX5" t="n">
         <v>-0.304784744977951</v>
       </c>
-      <c r="BX4" t="n">
+      <c r="BY5" t="n">
         <v>0.02694137394428253</v>
       </c>
-      <c r="BY4" t="n">
+      <c r="BZ5" t="n">
         <v>0.3864977359771729</v>
       </c>
-      <c r="BZ4" t="n">
+      <c r="CA5" t="n">
         <v>0.1446642726659775</v>
       </c>
-      <c r="CA4" t="n">
+      <c r="CB5" t="n">
         <v>-0.1520258486270905</v>
       </c>
-      <c r="CB4" t="n">
+      <c r="CC5" t="n">
         <v>0.08836635947227478</v>
       </c>
-      <c r="CC4" t="n">
+      <c r="CD5" t="n">
         <v>-0.04046059027314186</v>
       </c>
-      <c r="CD4" t="n">
+      <c r="CE5" t="n">
         <v>0.03495679795742035</v>
       </c>
-      <c r="CE4" t="n">
+      <c r="CF5" t="n">
         <v>0.1301746070384979</v>
       </c>
-      <c r="CF4" t="n">
+      <c r="CG5" t="n">
         <v>0.1207738593220711</v>
       </c>
-      <c r="CG4" t="n">
+      <c r="CH5" t="n">
         <v>-0.04280385002493858</v>
       </c>
-      <c r="CH4" t="n">
+      <c r="CI5" t="n">
         <v>0.06248047947883606</v>
       </c>
-      <c r="CI4" t="n">
+      <c r="CJ5" t="n">
         <v>-0.1344617754220963</v>
       </c>
-      <c r="CJ4" t="n">
+      <c r="CK5" t="n">
         <v>0.05777309834957123</v>
       </c>
-      <c r="CK4" t="n">
+      <c r="CL5" t="n">
         <v>0.245211586356163</v>
       </c>
-      <c r="CL4" t="n">
+      <c r="CM5" t="n">
         <v>-0.08524768799543381</v>
       </c>
-      <c r="CM4" t="n">
+      <c r="CN5" t="n">
         <v>-0.02847550250589848</v>
       </c>
-      <c r="CN4" t="n">
+      <c r="CO5" t="n">
         <v>0.1869578510522842</v>
       </c>
-      <c r="CO4" t="n">
+      <c r="CP5" t="n">
         <v>0.05987383425235748</v>
       </c>
-      <c r="CP4" t="n">
+      <c r="CQ5" t="n">
         <v>0.1164320111274719</v>
       </c>
-      <c r="CQ4" t="n">
+      <c r="CR5" t="n">
         <v>0.04716560244560242</v>
       </c>
-      <c r="CR4" t="n">
+      <c r="CS5" t="n">
         <v>0.01386433839797974</v>
       </c>
-      <c r="CS4" t="n">
+      <c r="CT5" t="n">
         <v>-0.02070973813533783</v>
       </c>
-      <c r="CT4" t="n">
+      <c r="CU5" t="n">
         <v>0.01532096788287163</v>
       </c>
-      <c r="CU4" t="n">
+      <c r="CV5" t="n">
         <v>-0.1451727598905563</v>
       </c>
-      <c r="CV4" t="n">
+      <c r="CW5" t="n">
         <v>0.03620017319917679</v>
       </c>
-      <c r="CW4" t="n">
+      <c r="CX5" t="n">
         <v>0.09348283708095551</v>
       </c>
-      <c r="CX4" t="n">
+      <c r="CY5" t="n">
         <v>-0.004446474835276604</v>
       </c>
-      <c r="CY4" t="n">
+      <c r="CZ5" t="n">
         <v>0.002868473529815674</v>
       </c>
-      <c r="CZ4" t="n">
+      <c r="DA5" t="n">
         <v>0.06505899876356125</v>
       </c>
-      <c r="DA4" t="n">
+      <c r="DB5" t="n">
         <v>-0.1446656286716461</v>
       </c>
-      <c r="DB4" t="n">
+      <c r="DC5" t="n">
         <v>0.1354619413614273</v>
       </c>
-      <c r="DC4" t="n">
+      <c r="DD5" t="n">
         <v>-0.02313166856765747</v>
       </c>
-      <c r="DD4" t="n">
+      <c r="DE5" t="n">
         <v>0.03633891046047211</v>
       </c>
-      <c r="DE4" t="n">
+      <c r="DF5" t="n">
         <v>0.04738517850637436</v>
       </c>
-      <c r="DF4" t="n">
+      <c r="DG5" t="n">
         <v>-0.06536491215229034</v>
       </c>
-      <c r="DG4" t="n">
+      <c r="DH5" t="n">
         <v>-0.1013645827770233</v>
       </c>
-      <c r="DH4" t="n">
+      <c r="DI5" t="n">
         <v>-0.05722665786743164</v>
       </c>
-      <c r="DI4" t="n">
+      <c r="DJ5" t="n">
         <v>0.0991760790348053</v>
       </c>
-      <c r="DJ4" t="n">
+      <c r="DK5" t="n">
         <v>-0.1798270493745804</v>
       </c>
-      <c r="DK4" t="n">
+      <c r="DL5" t="n">
         <v>0.1431812345981598</v>
       </c>
-      <c r="DL4" t="n">
+      <c r="DM5" t="n">
         <v>0.1779062151908875</v>
       </c>
-      <c r="DM4" t="n">
+      <c r="DN5" t="n">
         <v>0.0675027146935463</v>
       </c>
-      <c r="DN4" t="n">
+      <c r="DO5" t="n">
         <v>0.1118984892964363</v>
       </c>
-      <c r="DO4" t="n">
+      <c r="DP5" t="n">
         <v>0.1660496443510056</v>
       </c>
-      <c r="DP4" t="n">
+      <c r="DQ5" t="n">
         <v>0.04290303587913513</v>
       </c>
-      <c r="DQ4" t="n">
+      <c r="DR5" t="n">
         <v>-0.0223298966884613</v>
       </c>
-      <c r="DR4" t="n">
+      <c r="DS5" t="n">
         <v>0.02490139007568359</v>
       </c>
-      <c r="DS4" t="n">
+      <c r="DT5" t="n">
         <v>-0.2426488995552063</v>
       </c>
-      <c r="DT4" t="n">
+      <c r="DU5" t="n">
         <v>-0.01144071202725172</v>
       </c>
-      <c r="DU4" t="n">
+      <c r="DV5" t="n">
         <v>0.1421199440956116</v>
       </c>
-      <c r="DV4" t="n">
+      <c r="DW5" t="n">
         <v>-0.004106044769287109</v>
       </c>
-      <c r="DW4" t="n">
+      <c r="DX5" t="n">
         <v>0.08463555574417114</v>
       </c>
-      <c r="DX4" t="n">
+      <c r="DY5" t="n">
         <v>0.01743845269083977</v>
       </c>
     </row>

</xml_diff>